<commit_message>
Substantially updated these with definitions, domains and ranges, spelling corrections and new classes
</commit_message>
<xml_diff>
--- a/resources/OntologyTopLevelDefinitions.xlsx
+++ b/resources/OntologyTopLevelDefinitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\divitag2\work\softwareRepos\framework-legacy\01_Sandboxes\850_emfo_utilities\85_01_resources\src\main\resources\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\divitag2\work\softwareRepos\EcologicalMentalFunctioningOntology\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894854A6-2620-4307-8199-56A47A7D28E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745472EE-537C-4F5B-9AC5-7C86023ADFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40125" yWindow="795" windowWidth="23970" windowHeight="12870" tabRatio="463" xr2:uid="{9A7D1081-669E-4486-97AA-E16A917A201B}"/>
+    <workbookView xWindow="29430" yWindow="2535" windowWidth="26295" windowHeight="11940" tabRatio="463" xr2:uid="{9A7D1081-669E-4486-97AA-E16A917A201B}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="647">
   <si>
     <t>Ontology ID</t>
   </si>
@@ -2766,9 +2766,6 @@
     <t>EMFO_C013472</t>
   </si>
   <si>
-    <t>Observable_Behavior</t>
-  </si>
-  <si>
     <t>Behavior observable</t>
   </si>
   <si>
@@ -3013,6 +3010,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Problems in </t>
@@ -3023,6 +3021,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>mental</t>
@@ -3032,6 +3031,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> body function or structure as a result of significant deviation or loss (ICF, 2001).</t>
@@ -3645,6 +3645,372 @@
     <t xml:space="preserve">These include tangible features within the immediate space one occupies.  These features surround the person proximally and include: (1) physical environments (natural world; human-made objects, technology, and built structures), and (2) social environments made up of other people or animals that provide practical physical or emotional support, and includes the attitudes of others toward the person (open, friendly, prejudice, etc.).  (Brandt  and  Pope, 1997, ICF, 2001).  
 Environmental factors are dynamic and impact and exert influence directly upon the person and their behavior occurring moment by moment, and over time.  They are more malleable for the person to influence and shape due to the direct transactional relationship that exists between the person and their physical and social environments. 
 </t>
+  </si>
+  <si>
+    <t>Functioning_Performance</t>
+  </si>
+  <si>
+    <t>Performance_Metrics</t>
+  </si>
+  <si>
+    <t>Independence</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Assistance</t>
+  </si>
+  <si>
+    <t>Disability_Status</t>
+  </si>
+  <si>
+    <t>External_Factors_Metrics</t>
+  </si>
+  <si>
+    <t>Barriers</t>
+  </si>
+  <si>
+    <t>Facilitators</t>
+  </si>
+  <si>
+    <t>Person_Metrics</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Imparment</t>
+  </si>
+  <si>
+    <t>Limitation</t>
+  </si>
+  <si>
+    <t>Cognitive_Level</t>
+  </si>
+  <si>
+    <t>EMFO_C622689</t>
+  </si>
+  <si>
+    <t>EMFO_C283254</t>
+  </si>
+  <si>
+    <t>EMFO_C149655</t>
+  </si>
+  <si>
+    <t>EMFO_C662842</t>
+  </si>
+  <si>
+    <t>EMFO_C237030</t>
+  </si>
+  <si>
+    <t>EMFO_C735541</t>
+  </si>
+  <si>
+    <t>EMFO_C175985</t>
+  </si>
+  <si>
+    <t>EMFO_C907771</t>
+  </si>
+  <si>
+    <t>EMFO_C161386</t>
+  </si>
+  <si>
+    <t>EMFO_C855770</t>
+  </si>
+  <si>
+    <t>EMFO_C312100</t>
+  </si>
+  <si>
+    <t>EMFO_C154803</t>
+  </si>
+  <si>
+    <t>EMFO_C028229</t>
+  </si>
+  <si>
+    <t>EMFO_C087536</t>
+  </si>
+  <si>
+    <t>EMFO_C236637</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000015#process</t>
+  </si>
+  <si>
+    <t>Functioning</t>
+  </si>
+  <si>
+    <t>Function-ing</t>
+  </si>
+  <si>
+    <t>EMFO_C322443</t>
+  </si>
+  <si>
+    <t>Self_Reported_Functioning</t>
+  </si>
+  <si>
+    <t>Observed_Behavior</t>
+  </si>
+  <si>
+    <t>Functioning_Observed_By_Others</t>
+  </si>
+  <si>
+    <t>EMFO_C870384</t>
+  </si>
+  <si>
+    <t>continuant</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000004</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000004#independent_continuant_continuant</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000017#Realizable_Entity</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000020#specifically_dependent_continuant</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000002#continuant</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000017</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000020</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000002</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000001</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000001#entity</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000016</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000016#disposition</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000034</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000034#function</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000015</t>
+  </si>
+  <si>
+    <t>obo:BFO_0000003#occurrent</t>
+  </si>
+  <si>
+    <t>In all areas of empirical inquiry we encounter general terms of two sorts. First are general terms which refer to universals or types:animaltuberculosissurgical procedurediseaseSecond, are general terms used to refer to groups of entities which instantiate a given universal but do not correspond to the extension of any subuniversal of that universal because there is nothing intrinsic to the entities in question by virtue of which they – and only they – are counted as belonging to the given group. Examples are: animal purchased by the Emperortuberculosis diagnosed on a Wednesdaysurgical procedure performed on a patient from Stockholmperson identified as candidate for clinical trial #2056-555person who is signatory of Form 656-PPVpainting by Leonardo da VinciSuch terms, which represent what are called ‘specializations’ in [81</t>
+  </si>
+  <si>
+    <t>BFO 2 Reference: Continuant entities are entities which can be sliced to yield parts only along the spatial dimension, yielding for example the parts of your table which we call its legs, its top, its nails. ‘My desk stretches from the window to the door. It has spatial parts, and can be sliced (in space) in two. With respect to time, however, a thing is a continuant.’ [60, p. 240</t>
+  </si>
+  <si>
+    <t>b is an independent continuant = Def. b is a continuant which is such that there is no c and no t such that b s-depends_on c at t. (axiom label in BFO2 Reference: [017-002])</t>
+  </si>
+  <si>
+    <t>b is a specifically dependent continuant = Def. b is a continuant &amp; there is some independent continuant c which is not a spatial region and which is such that b s-depends_on c at every time t during the course of b’s existence. (axiom label in BFO2 Reference: [050-003])</t>
+  </si>
+  <si>
+    <t>To say that b is a realizable entity is to say that b is a specifically dependent continuant that inheres in some independent continuant which is not a spatial region and is of a type instances of which are realized in processes of a correlated type. (axiom label in BFO2 Reference: [058-002])</t>
+  </si>
+  <si>
+    <t>b is a disposition means: b is a realizable entity &amp; b’s bearer is some material entity &amp; b is such that if it ceases to exist, then its bearer is physically changed, &amp; b’s realization occurs when and because this bearer is in some special physical circumstances, &amp; this realization occurs in virtue of the bearer’s physical make-up. (axiom label in BFO2 Reference: [062-002])</t>
+  </si>
+  <si>
+    <t>A function is a disposition that exists in virtue of the bearer’s physical make-up and this physical make-up is something the bearer possesses because it came into being, either through evolution (in the case of natural biological entities) or through intentional design (in the case of artifacts), in order to realize processes of a certain sort. (axiom label in BFO2 Reference: [064-001])</t>
+  </si>
+  <si>
+    <t>p is a process = Def. p is an occurrent that has temporal proper parts and for some time t, p s-depends_on some material entity at t. (axiom label in BFO2 Reference: [083-003])</t>
+  </si>
+  <si>
+    <t>EMFO_C573853</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>Observer</t>
+  </si>
+  <si>
+    <t>Person under a clinician's care</t>
+  </si>
+  <si>
+    <t>Clinician</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observer </t>
+  </si>
+  <si>
+    <t>A professional having direct contact with patients</t>
+  </si>
+  <si>
+    <t>EMFO_C895326</t>
+  </si>
+  <si>
+    <t>EMFO_C603221</t>
+  </si>
+  <si>
+    <t>EMFO_C335152</t>
+  </si>
+  <si>
+    <t>Lived_Experience_Of_Participation</t>
+  </si>
+  <si>
+    <t>EMFO_C418571</t>
+  </si>
+  <si>
+    <t>Social Environment</t>
+  </si>
+  <si>
+    <t>EMFO_C712863</t>
+  </si>
+  <si>
+    <t>Physical_Environment</t>
+  </si>
+  <si>
+    <t>EMFO_D964857</t>
+  </si>
+  <si>
+    <t>EMFO_D601365</t>
+  </si>
+  <si>
+    <t>EMFO_D376411</t>
+  </si>
+  <si>
+    <t>EMFO_D680170</t>
+  </si>
+  <si>
+    <t>EMFO_D148915</t>
+  </si>
+  <si>
+    <t>EMFO_D902639</t>
+  </si>
+  <si>
+    <t>EMFO_D497531</t>
+  </si>
+  <si>
+    <t>EMFO_D482275</t>
+  </si>
+  <si>
+    <t>EMFO_D934806</t>
+  </si>
+  <si>
+    <t>EMFO_D114490</t>
+  </si>
+  <si>
+    <t>EMFO_D582362</t>
+  </si>
+  <si>
+    <t>EMFO_D535704</t>
+  </si>
+  <si>
+    <t>EMFO_D262389</t>
+  </si>
+  <si>
+    <t>EMFO_D946246</t>
+  </si>
+  <si>
+    <t>EMFO_D840452</t>
+  </si>
+  <si>
+    <t>EMFO_D416705</t>
+  </si>
+  <si>
+    <t>EMFO_D444569</t>
+  </si>
+  <si>
+    <t>EMFO_D092995</t>
+  </si>
+  <si>
+    <t>EMFO_D595504</t>
+  </si>
+  <si>
+    <t>EMFO_D048813</t>
+  </si>
+  <si>
+    <t>EMFO_D998417</t>
+  </si>
+  <si>
+    <t>EMFO_D828787</t>
+  </si>
+  <si>
+    <t>EMFO_D571934</t>
+  </si>
+  <si>
+    <t>EMFO_D151384</t>
+  </si>
+  <si>
+    <t>EMFO_D502022</t>
+  </si>
+  <si>
+    <t>EMFO_D333215</t>
+  </si>
+  <si>
+    <t>EMFO_D534508</t>
+  </si>
+  <si>
+    <t>EMFO_D880054</t>
+  </si>
+  <si>
+    <t>EMFO_D747279</t>
+  </si>
+  <si>
+    <t>EMFO_D268654</t>
+  </si>
+  <si>
+    <t>EMFO_D286629</t>
+  </si>
+  <si>
+    <t>EMFO_D603963</t>
+  </si>
+  <si>
+    <t>EMFO_D004636</t>
+  </si>
+  <si>
+    <t>EMFO_D512242</t>
+  </si>
+  <si>
+    <t>EMFO_D206896</t>
+  </si>
+  <si>
+    <t>EMFO_D131405</t>
+  </si>
+  <si>
+    <t>EMFO_D349244</t>
+  </si>
+  <si>
+    <t>EMFO_D999870</t>
+  </si>
+  <si>
+    <t>EMFO_D343431</t>
+  </si>
+  <si>
+    <t>EMFO_D018110</t>
+  </si>
+  <si>
+    <t>EMFO_D513641</t>
+  </si>
+  <si>
+    <t>EMFO_D953520</t>
+  </si>
+  <si>
+    <t>EMFO_D643924</t>
+  </si>
+  <si>
+    <t>Distal_Contextual_Factors</t>
+  </si>
+  <si>
+    <t>Proximal_Contextual_Factors</t>
   </si>
 </sst>
 </file>
@@ -3788,6 +4154,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3795,6 +4162,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3805,7 +4173,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3881,6 +4249,30 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB686DA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -3936,7 +4328,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4070,6 +4462,13 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -4081,6 +4480,11 @@
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{9274D3CB-DAB3-4C4B-9DF6-A69604A0D4A9}"/>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFB686DA"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4159,9 +4563,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4199,7 +4603,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4305,7 +4709,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4447,7 +4851,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4458,19 +4862,19 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:W88"/>
+  <dimension ref="A1:W119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B59" sqref="B59"/>
+      <selection pane="bottomRight" activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="26.7109375" style="15" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" style="15" customWidth="1"/>
+    <col min="3" max="3" width="51.140625" style="15" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" style="15" customWidth="1"/>
     <col min="5" max="5" width="26.28515625" style="15" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" style="15" customWidth="1"/>
@@ -4495,7 +4899,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>0</v>
@@ -4566,13 +4970,13 @@
     </row>
     <row r="2" spans="1:23" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
+        <v>495</v>
+      </c>
+      <c r="B2" t="s">
+        <v>475</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>496</v>
-      </c>
-      <c r="B2" t="s">
-        <v>476</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>497</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15" t="s">
@@ -4615,7 +5019,7 @@
     </row>
     <row r="3" spans="1:23" ht="153" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>28</v>
@@ -4625,7 +5029,7 @@
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="17" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>30</v>
@@ -4664,13 +5068,13 @@
     </row>
     <row r="4" spans="1:23" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15" t="s">
@@ -4699,13 +5103,13 @@
     </row>
     <row r="5" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>38</v>
@@ -4738,13 +5142,13 @@
     </row>
     <row r="6" spans="1:23" s="16" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B6" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15" t="s">
@@ -4791,13 +5195,13 @@
     </row>
     <row r="7" spans="1:23" ht="165.75" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>51</v>
@@ -4830,13 +5234,13 @@
     </row>
     <row r="8" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>50</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15" t="s">
@@ -4867,13 +5271,13 @@
     </row>
     <row r="9" spans="1:23" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>61</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15" t="s">
@@ -4916,13 +5320,13 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>66</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>67</v>
@@ -4940,13 +5344,13 @@
     </row>
     <row r="11" spans="1:23" ht="191.25" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16" t="s">
@@ -4993,7 +5397,7 @@
     </row>
     <row r="12" spans="1:23" s="16" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>77</v>
@@ -5052,13 +5456,13 @@
     </row>
     <row r="13" spans="1:23" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>84</v>
@@ -5070,7 +5474,7 @@
         <v>86</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11" t="s">
@@ -5095,13 +5499,13 @@
     </row>
     <row r="14" spans="1:23" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B14" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15" t="s">
@@ -5130,13 +5534,13 @@
     </row>
     <row r="15" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B15" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>90</v>
@@ -5152,13 +5556,13 @@
     </row>
     <row r="16" spans="1:23" s="16" customFormat="1" ht="89.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B16" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11" t="s">
@@ -5205,13 +5609,13 @@
     </row>
     <row r="17" spans="1:23" ht="204" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>99</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>100</v>
@@ -5250,13 +5654,13 @@
     </row>
     <row r="18" spans="1:23" ht="242.25" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>106</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16" t="s">
@@ -5266,7 +5670,7 @@
         <v>108</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H18" s="17" t="s">
         <v>109</v>
@@ -5303,13 +5707,13 @@
     </row>
     <row r="19" spans="1:23" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16" t="s">
@@ -5356,7 +5760,7 @@
     </row>
     <row r="20" spans="1:23" s="16" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>117</v>
@@ -5392,13 +5796,13 @@
     </row>
     <row r="21" spans="1:23" ht="51" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>124</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="17" t="s">
@@ -5431,13 +5835,13 @@
     </row>
     <row r="22" spans="1:23" s="16" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B22" s="45" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E22" s="16" t="s">
         <v>129</v>
@@ -5476,7 +5880,7 @@
     </row>
     <row r="23" spans="1:23" s="20" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>136</v>
@@ -5529,13 +5933,13 @@
     </row>
     <row r="24" spans="1:23" s="16" customFormat="1" ht="102" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E24" s="16" t="s">
         <v>143</v>
@@ -5565,13 +5969,13 @@
     </row>
     <row r="25" spans="1:23" ht="51" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="17" t="s">
@@ -5616,13 +6020,13 @@
     </row>
     <row r="26" spans="1:23" s="16" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>153</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E26" s="16" t="s">
         <v>154</v>
@@ -5664,13 +6068,13 @@
     </row>
     <row r="27" spans="1:23" ht="102" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>160</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>161</v>
@@ -5703,7 +6107,7 @@
     </row>
     <row r="28" spans="1:23" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>166</v>
@@ -5721,7 +6125,7 @@
         <v>170</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I28" s="11"/>
       <c r="J28" s="11" t="s">
@@ -5745,13 +6149,13 @@
     </row>
     <row r="29" spans="1:23" s="16" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="16" t="s">
@@ -5764,7 +6168,7 @@
         <v>174</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I29" s="17"/>
       <c r="J29" s="27" t="s">
@@ -5791,13 +6195,13 @@
     </row>
     <row r="30" spans="1:23" ht="51" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B30" s="46" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E30" s="15" t="s">
         <v>178</v>
@@ -5833,13 +6237,13 @@
     </row>
     <row r="31" spans="1:23" s="16" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E31" s="16" t="s">
         <v>183</v>
@@ -5875,7 +6279,7 @@
     </row>
     <row r="32" spans="1:23" ht="51" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>188</v>
@@ -5924,7 +6328,7 @@
     </row>
     <row r="33" spans="1:23" s="16" customFormat="1" ht="102" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>196</v>
@@ -5973,7 +6377,7 @@
     </row>
     <row r="34" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>201</v>
@@ -6016,13 +6420,13 @@
     </row>
     <row r="35" spans="1:23" s="16" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>209</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E35" s="16" t="s">
         <v>210</v>
@@ -6068,13 +6472,13 @@
     </row>
     <row r="36" spans="1:23" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B36" s="21" t="s">
         <v>209</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="17" t="s">
@@ -6109,13 +6513,13 @@
     </row>
     <row r="37" spans="1:23" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B37" s="45" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E37" s="15" t="s">
         <v>220</v>
@@ -6151,13 +6555,13 @@
     </row>
     <row r="38" spans="1:23" s="16" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B38" s="45" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E38" s="16" t="s">
         <v>226</v>
@@ -6196,13 +6600,13 @@
     </row>
     <row r="39" spans="1:23" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B39" s="46" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E39" s="32" t="s">
         <v>232</v>
@@ -6241,7 +6645,7 @@
     </row>
     <row r="40" spans="1:23" s="16" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B40" s="21" t="s">
         <v>239</v>
@@ -6277,7 +6681,7 @@
     </row>
     <row r="41" spans="1:23" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B41" s="33" t="s">
         <v>245</v>
@@ -6289,15 +6693,15 @@
         <v>247</v>
       </c>
       <c r="G41" s="44" t="s">
+        <v>472</v>
+      </c>
+      <c r="H41" s="44" t="s">
         <v>473</v>
-      </c>
-      <c r="H41" s="44" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="42" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B42" s="34" t="s">
         <v>248</v>
@@ -6317,7 +6721,7 @@
     </row>
     <row r="43" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B43" s="34" t="s">
         <v>253</v>
@@ -6350,625 +6754,625 @@
     </row>
     <row r="44" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B44" s="34" t="s">
         <v>261</v>
       </c>
       <c r="C44" s="34" t="s">
-        <v>262</v>
+        <v>559</v>
       </c>
       <c r="D44" s="34" t="s">
         <v>189</v>
       </c>
       <c r="E44" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="F44" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="G44" s="11" t="s">
         <v>264</v>
-      </c>
-      <c r="G44" s="11" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="45" spans="1:23" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B45" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="C45" s="34" t="s">
         <v>266</v>
       </c>
-      <c r="C45" s="34" t="s">
+      <c r="D45" s="34" t="s">
         <v>267</v>
       </c>
-      <c r="D45" s="34" t="s">
+      <c r="E45" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="F45" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="F45" s="15" t="s">
+      <c r="G45" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="G45" s="11" t="s">
-        <v>271</v>
-      </c>
       <c r="H45" s="11" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I45" s="11"/>
     </row>
     <row r="46" spans="1:23" ht="51" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B46" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="C46" s="34" t="s">
         <v>272</v>
       </c>
-      <c r="C46" s="34" t="s">
+      <c r="D46" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="D46" s="34" t="s">
-        <v>268</v>
-      </c>
-      <c r="E46" s="11" t="s">
+      <c r="F46" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="F46" s="15" t="s">
+      <c r="G46" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="G46" s="11" t="s">
+      <c r="H46" s="11" t="s">
         <v>276</v>
-      </c>
-      <c r="H46" s="11" t="s">
-        <v>277</v>
       </c>
       <c r="I46" s="11"/>
     </row>
     <row r="47" spans="1:23" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B47" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="C47" s="34" t="s">
         <v>278</v>
       </c>
-      <c r="C47" s="34" t="s">
+      <c r="D47" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="E47" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="D47" s="34" t="s">
-        <v>268</v>
-      </c>
-      <c r="E47" s="15" t="s">
+      <c r="F47" s="41" t="s">
         <v>280</v>
       </c>
-      <c r="F47" s="41" t="s">
+      <c r="G47" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="G47" s="11" t="s">
+      <c r="H47" s="11" t="s">
         <v>282</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>283</v>
       </c>
       <c r="I47" s="11"/>
     </row>
     <row r="48" spans="1:23" ht="51" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B48" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="C48" s="34" t="s">
         <v>284</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="D48" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="G48" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="D48" s="34" t="s">
-        <v>268</v>
-      </c>
-      <c r="G48" s="11" t="s">
+      <c r="H48" s="11" t="s">
         <v>286</v>
-      </c>
-      <c r="H48" s="11" t="s">
-        <v>287</v>
       </c>
       <c r="I48" s="11"/>
     </row>
     <row r="49" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B49" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="C49" s="34" t="s">
         <v>288</v>
       </c>
-      <c r="C49" s="34" t="s">
+      <c r="D49" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="G49" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="D49" s="34" t="s">
-        <v>268</v>
-      </c>
-      <c r="G49" s="11" t="s">
+      <c r="H49" s="11" t="s">
         <v>290</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>291</v>
       </c>
       <c r="I49" s="11"/>
     </row>
     <row r="50" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B50" s="34" t="s">
+        <v>291</v>
+      </c>
+      <c r="C50" s="34" t="s">
         <v>292</v>
       </c>
-      <c r="C50" s="34" t="s">
+      <c r="D50" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="G50" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="D50" s="34" t="s">
-        <v>268</v>
-      </c>
-      <c r="G50" s="11" t="s">
+      <c r="H50" s="11" t="s">
         <v>294</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>295</v>
       </c>
       <c r="I50" s="11"/>
     </row>
     <row r="51" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B51" s="34" t="s">
+        <v>295</v>
+      </c>
+      <c r="C51" s="34" t="s">
         <v>296</v>
       </c>
-      <c r="C51" s="34" t="s">
+      <c r="D51" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="G51" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="D51" s="34" t="s">
-        <v>268</v>
-      </c>
-      <c r="G51" s="11" t="s">
+      <c r="H51" s="11" t="s">
         <v>298</v>
-      </c>
-      <c r="H51" s="11" t="s">
-        <v>299</v>
       </c>
       <c r="I51" s="11"/>
     </row>
     <row r="52" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B52" s="34" t="s">
+        <v>299</v>
+      </c>
+      <c r="C52" s="34" t="s">
         <v>300</v>
       </c>
-      <c r="C52" s="34" t="s">
+      <c r="D52" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="G52" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="D52" s="34" t="s">
-        <v>268</v>
-      </c>
-      <c r="G52" s="11" t="s">
+      <c r="H52" s="11" t="s">
         <v>302</v>
-      </c>
-      <c r="H52" s="11" t="s">
-        <v>303</v>
       </c>
       <c r="I52" s="11"/>
     </row>
     <row r="53" spans="1:9" ht="204" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B53" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="C53" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="C53" s="34" t="s">
-        <v>305</v>
-      </c>
       <c r="D53" s="34" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F53" s="11"/>
       <c r="G53" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="H53" s="11" t="s">
         <v>306</v>
-      </c>
-      <c r="H53" s="11" t="s">
-        <v>307</v>
       </c>
       <c r="I53" s="11"/>
     </row>
     <row r="54" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B54" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="C54" s="34" t="s">
         <v>308</v>
       </c>
-      <c r="C54" s="34" t="s">
+      <c r="D54" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D54" s="34" t="s">
+      <c r="G54" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="G54" s="11" t="s">
+      <c r="H54" s="11" t="s">
         <v>311</v>
-      </c>
-      <c r="H54" s="11" t="s">
-        <v>312</v>
       </c>
       <c r="I54" s="11"/>
     </row>
     <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B55" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="C55" s="35" t="s">
         <v>313</v>
       </c>
-      <c r="C55" s="35" t="s">
+      <c r="D55" s="34" t="s">
         <v>314</v>
       </c>
-      <c r="D55" s="34" t="s">
+      <c r="G55" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="G55" s="11" t="s">
+      <c r="H55" s="15" t="s">
         <v>316</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B56" s="34" t="s">
+        <v>317</v>
+      </c>
+      <c r="C56" s="34" t="s">
         <v>318</v>
       </c>
-      <c r="C56" s="34" t="s">
+      <c r="D56" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="G56" s="11" t="s">
         <v>319</v>
-      </c>
-      <c r="D56" s="34" t="s">
-        <v>315</v>
-      </c>
-      <c r="G56" s="11" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B57" s="34" t="s">
+        <v>320</v>
+      </c>
+      <c r="C57" s="34" t="s">
         <v>321</v>
       </c>
-      <c r="C57" s="34" t="s">
+      <c r="D57" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="G57" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="D57" s="34" t="s">
-        <v>315</v>
-      </c>
-      <c r="G57" s="11" t="s">
+      <c r="H57" s="15" t="s">
         <v>323</v>
-      </c>
-      <c r="H57" s="15" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B58" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="C58" s="35" t="s">
         <v>325</v>
       </c>
-      <c r="C58" s="35" t="s">
+      <c r="D58" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="G58" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="D58" s="34" t="s">
-        <v>315</v>
-      </c>
-      <c r="G58" s="11" t="s">
-        <v>327</v>
-      </c>
       <c r="H58" s="15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B59" s="45" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C59" s="35" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D59" s="34"/>
       <c r="G59" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="H59" s="15" t="s">
         <v>328</v>
-      </c>
-      <c r="H59" s="15" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B60" s="45" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C60" s="35" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D60" s="34"/>
       <c r="G60" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="H60" s="11" t="s">
         <v>330</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B61" s="46" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C61" s="35" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D61" s="34"/>
       <c r="G61" s="11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B62" s="46" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C62" s="35" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D62" s="34"/>
       <c r="G62" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B63" s="46" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D63" s="34"/>
       <c r="G63" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="H63" s="15" t="s">
         <v>334</v>
-      </c>
-      <c r="H63" s="15" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B64" s="36" t="s">
+        <v>335</v>
+      </c>
+      <c r="C64" s="36" t="s">
         <v>336</v>
       </c>
-      <c r="C64" s="36" t="s">
+      <c r="D64" s="36" t="s">
+        <v>309</v>
+      </c>
+      <c r="E64" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="D64" s="36" t="s">
-        <v>310</v>
-      </c>
-      <c r="E64" s="11" t="s">
+      <c r="F64" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="F64" s="11" t="s">
+      <c r="G64" s="42" t="s">
         <v>339</v>
       </c>
-      <c r="G64" s="42" t="s">
+      <c r="H64" s="11" t="s">
         <v>340</v>
-      </c>
-      <c r="H64" s="11" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B65" s="36" t="s">
+        <v>341</v>
+      </c>
+      <c r="C65" s="36" t="s">
         <v>342</v>
       </c>
-      <c r="C65" s="36" t="s">
+      <c r="D65" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="D65" s="36" t="s">
+      <c r="E65" s="15" t="s">
+        <v>441</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>440</v>
+      </c>
+      <c r="G65" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="E65" s="15" t="s">
-        <v>442</v>
-      </c>
-      <c r="F65" s="15" t="s">
-        <v>441</v>
-      </c>
-      <c r="G65" s="11" t="s">
+      <c r="H65" s="11" t="s">
         <v>345</v>
-      </c>
-      <c r="H65" s="11" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B66" s="36" t="s">
+        <v>346</v>
+      </c>
+      <c r="C66" s="36" t="s">
         <v>347</v>
       </c>
-      <c r="C66" s="36" t="s">
-        <v>348</v>
-      </c>
       <c r="D66" s="36" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E66" s="15" t="s">
+        <v>442</v>
+      </c>
+      <c r="F66" s="15" t="s">
         <v>443</v>
       </c>
-      <c r="F66" s="15" t="s">
-        <v>444</v>
-      </c>
       <c r="G66" s="11" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H66" s="43"/>
     </row>
     <row r="67" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B67" s="36" t="s">
+        <v>348</v>
+      </c>
+      <c r="C67" s="36" t="s">
         <v>349</v>
       </c>
-      <c r="C67" s="36" t="s">
+      <c r="D67" s="36" t="s">
         <v>350</v>
       </c>
-      <c r="D67" s="36" t="s">
-        <v>351</v>
-      </c>
       <c r="E67" s="15" t="s">
+        <v>451</v>
+      </c>
+      <c r="F67" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="G67" s="11" t="s">
         <v>452</v>
       </c>
-      <c r="F67" s="15" t="s">
-        <v>451</v>
-      </c>
-      <c r="G67" s="11" t="s">
+      <c r="H67" s="11" t="s">
         <v>453</v>
-      </c>
-      <c r="H67" s="11" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B68" s="36" t="s">
+        <v>351</v>
+      </c>
+      <c r="C68" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="C68" s="36" t="s">
+      <c r="D68" s="36" t="s">
         <v>353</v>
       </c>
-      <c r="D68" s="36" t="s">
+      <c r="E68" s="15" t="s">
         <v>354</v>
       </c>
-      <c r="E68" s="15" t="s">
+      <c r="F68" s="15" t="s">
         <v>355</v>
-      </c>
-      <c r="F68" s="15" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B69" s="36" t="s">
+        <v>356</v>
+      </c>
+      <c r="C69" s="36" t="s">
         <v>357</v>
       </c>
-      <c r="C69" s="36" t="s">
+      <c r="D69" s="36" t="s">
+        <v>352</v>
+      </c>
+      <c r="E69" s="15" t="s">
         <v>358</v>
       </c>
-      <c r="D69" s="36" t="s">
-        <v>353</v>
-      </c>
-      <c r="E69" s="15" t="s">
+      <c r="F69" s="15" t="s">
         <v>359</v>
       </c>
-      <c r="F69" s="15" t="s">
+      <c r="G69" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="G69" s="11" t="s">
+      <c r="H69" s="15" t="s">
         <v>361</v>
       </c>
-      <c r="H69" s="15" t="s">
+      <c r="J69" s="15" t="s">
         <v>362</v>
       </c>
-      <c r="J69" s="15" t="s">
+      <c r="K69" s="15" t="s">
         <v>363</v>
-      </c>
-      <c r="K69" s="15" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="70" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B70" s="36" t="s">
+        <v>364</v>
+      </c>
+      <c r="C70" s="36" t="s">
         <v>365</v>
       </c>
-      <c r="C70" s="36" t="s">
-        <v>366</v>
-      </c>
       <c r="D70" s="36" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B71" s="36" t="s">
+        <v>366</v>
+      </c>
+      <c r="C71" s="36" t="s">
         <v>367</v>
       </c>
-      <c r="C71" s="36" t="s">
-        <v>368</v>
-      </c>
       <c r="D71" s="36" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="72" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A72" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B72" s="36" t="s">
+        <v>368</v>
+      </c>
+      <c r="C72" s="36" t="s">
         <v>369</v>
       </c>
-      <c r="C72" s="36" t="s">
-        <v>370</v>
-      </c>
       <c r="D72" s="36" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A73" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B73" s="37" t="s">
         <v>136</v>
@@ -6980,53 +7384,53 @@
         <v>250</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B74" s="37" t="s">
+        <v>370</v>
+      </c>
+      <c r="C74" s="37" t="s">
         <v>371</v>
       </c>
-      <c r="C74" s="37" t="s">
+      <c r="D74" s="37" t="s">
         <v>372</v>
       </c>
-      <c r="D74" s="37" t="s">
+      <c r="E74" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="F74" s="15" t="s">
         <v>373</v>
       </c>
-      <c r="E74" s="15" t="s">
-        <v>372</v>
-      </c>
-      <c r="F74" s="15" t="s">
+      <c r="G74" s="11" t="s">
         <v>374</v>
       </c>
-      <c r="G74" s="11" t="s">
+      <c r="H74" s="15" t="s">
         <v>375</v>
       </c>
-      <c r="H74" s="15" t="s">
+      <c r="J74" s="15" t="s">
         <v>376</v>
       </c>
-      <c r="J74" s="15" t="s">
+      <c r="K74" s="11" t="s">
         <v>377</v>
-      </c>
-      <c r="K74" s="11" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A75" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B75" s="37" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C75" s="37" t="s">
         <v>107</v>
       </c>
       <c r="D75" s="37" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E75" s="15" t="s">
         <v>107</v>
@@ -7035,13 +7439,13 @@
         <v>108</v>
       </c>
       <c r="G75" s="11" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H75" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="J75" s="15" t="s">
         <v>380</v>
-      </c>
-      <c r="J75" s="15" t="s">
-        <v>381</v>
       </c>
       <c r="K75" s="15" t="s">
         <v>260</v>
@@ -7049,215 +7453,215 @@
     </row>
     <row r="76" spans="1:11" ht="102" x14ac:dyDescent="0.25">
       <c r="A76" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B76" s="37" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C76" s="37" t="s">
+        <v>645</v>
+      </c>
+      <c r="D76" s="37" t="s">
         <v>383</v>
       </c>
-      <c r="D76" s="37" t="s">
-        <v>384</v>
-      </c>
       <c r="G76" s="11" t="s">
+        <v>467</v>
+      </c>
+      <c r="H76" s="11" t="s">
         <v>468</v>
-      </c>
-      <c r="H76" s="11" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
-        <v>496</v>
+        <v>602</v>
       </c>
       <c r="B77" s="37" t="s">
+        <v>384</v>
+      </c>
+      <c r="C77" s="37" t="s">
         <v>385</v>
       </c>
-      <c r="C77" s="37" t="s">
+      <c r="D77" s="37" t="s">
+        <v>383</v>
+      </c>
+      <c r="G77" s="11" t="s">
         <v>386</v>
       </c>
-      <c r="D77" s="37" t="s">
-        <v>384</v>
-      </c>
-      <c r="G77" s="11" t="s">
+      <c r="J77" s="15" t="s">
         <v>387</v>
-      </c>
-      <c r="J77" s="15" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
-        <v>496</v>
+        <v>603</v>
       </c>
       <c r="B78" s="37" t="s">
+        <v>388</v>
+      </c>
+      <c r="C78" s="37" t="s">
         <v>389</v>
       </c>
-      <c r="C78" s="37" t="s">
-        <v>390</v>
-      </c>
       <c r="D78" s="37" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="16" t="s">
-        <v>496</v>
+        <v>604</v>
       </c>
       <c r="B79" s="37" t="s">
+        <v>390</v>
+      </c>
+      <c r="C79" s="37" t="s">
         <v>391</v>
       </c>
-      <c r="C79" s="37" t="s">
-        <v>392</v>
-      </c>
       <c r="D79" s="37" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A80" s="16" t="s">
-        <v>496</v>
+        <v>605</v>
       </c>
       <c r="B80" s="37" t="s">
+        <v>392</v>
+      </c>
+      <c r="C80" s="37" t="s">
         <v>393</v>
       </c>
-      <c r="C80" s="37" t="s">
-        <v>394</v>
-      </c>
       <c r="D80" s="37" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
-        <v>496</v>
+        <v>606</v>
       </c>
       <c r="B81" s="37" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C81" s="37" t="s">
-        <v>396</v>
+        <v>646</v>
       </c>
       <c r="D81" s="37" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H81" s="11" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="16" t="s">
-        <v>496</v>
+        <v>607</v>
       </c>
       <c r="B82" s="37" t="s">
+        <v>396</v>
+      </c>
+      <c r="C82" s="37" t="s">
         <v>397</v>
       </c>
-      <c r="C82" s="37" t="s">
-        <v>398</v>
-      </c>
       <c r="D82" s="37" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H82" s="15" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A83" s="16" t="s">
-        <v>496</v>
+        <v>608</v>
       </c>
       <c r="B83" s="37" t="s">
+        <v>398</v>
+      </c>
+      <c r="C83" s="37" t="s">
         <v>399</v>
       </c>
-      <c r="C83" s="37" t="s">
-        <v>400</v>
-      </c>
       <c r="D83" s="37" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="16" t="s">
-        <v>496</v>
+        <v>609</v>
       </c>
       <c r="B84" s="37" t="s">
+        <v>400</v>
+      </c>
+      <c r="C84" s="37" t="s">
         <v>401</v>
       </c>
-      <c r="C84" s="37" t="s">
-        <v>402</v>
-      </c>
       <c r="D84" s="37" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="16" t="s">
-        <v>496</v>
+        <v>610</v>
       </c>
       <c r="B85" s="37" t="s">
+        <v>402</v>
+      </c>
+      <c r="C85" s="37" t="s">
         <v>403</v>
       </c>
-      <c r="C85" s="37" t="s">
+      <c r="D85" s="37" t="s">
         <v>404</v>
       </c>
-      <c r="D85" s="37" t="s">
-        <v>405</v>
-      </c>
       <c r="H85" s="15" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="16" t="s">
-        <v>496</v>
+        <v>611</v>
       </c>
       <c r="B86" s="37" t="s">
+        <v>405</v>
+      </c>
+      <c r="C86" s="37" t="s">
         <v>406</v>
       </c>
-      <c r="C86" s="37" t="s">
-        <v>407</v>
-      </c>
       <c r="D86" s="37" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H86" s="15" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="16" t="s">
-        <v>496</v>
+        <v>612</v>
       </c>
       <c r="B87" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="C87" s="38" t="s">
         <v>408</v>
-      </c>
-      <c r="C87" s="38" t="s">
-        <v>409</v>
       </c>
       <c r="D87" s="38" t="s">
         <v>118</v>
@@ -7265,16 +7669,474 @@
     </row>
     <row r="88" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="16" t="s">
-        <v>496</v>
+        <v>613</v>
       </c>
       <c r="B88" s="38" t="s">
+        <v>409</v>
+      </c>
+      <c r="C88" s="38" t="s">
         <v>410</v>
-      </c>
-      <c r="C88" s="38" t="s">
-        <v>411</v>
       </c>
       <c r="D88" s="38" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="15" t="s">
+        <v>614</v>
+      </c>
+      <c r="B89" s="47" t="s">
+        <v>539</v>
+      </c>
+      <c r="C89" s="47" t="s">
+        <v>556</v>
+      </c>
+      <c r="D89" s="46" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="15" t="s">
+        <v>615</v>
+      </c>
+      <c r="B90" s="47" t="s">
+        <v>540</v>
+      </c>
+      <c r="C90" s="47" t="s">
+        <v>525</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="15" t="s">
+        <v>616</v>
+      </c>
+      <c r="B91" s="47" t="s">
+        <v>541</v>
+      </c>
+      <c r="C91" s="47" t="s">
+        <v>526</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="15" t="s">
+        <v>617</v>
+      </c>
+      <c r="B92" s="47" t="s">
+        <v>542</v>
+      </c>
+      <c r="C92" s="47" t="s">
+        <v>527</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="15" t="s">
+        <v>618</v>
+      </c>
+      <c r="B93" s="48" t="s">
+        <v>543</v>
+      </c>
+      <c r="C93" s="48" t="s">
+        <v>528</v>
+      </c>
+      <c r="D93" s="15" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="15" t="s">
+        <v>619</v>
+      </c>
+      <c r="B94" s="48" t="s">
+        <v>544</v>
+      </c>
+      <c r="C94" s="48" t="s">
+        <v>529</v>
+      </c>
+      <c r="D94" s="15" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="B95" s="48" t="s">
+        <v>557</v>
+      </c>
+      <c r="C95" s="48" t="s">
+        <v>558</v>
+      </c>
+      <c r="D95" s="15" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B96" s="48" t="s">
+        <v>561</v>
+      </c>
+      <c r="C96" s="48" t="s">
+        <v>560</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="15" t="s">
+        <v>622</v>
+      </c>
+      <c r="B97" s="49" t="s">
+        <v>545</v>
+      </c>
+      <c r="C97" s="49" t="s">
+        <v>530</v>
+      </c>
+      <c r="D97" s="15" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="15" t="s">
+        <v>623</v>
+      </c>
+      <c r="B98" s="50" t="s">
+        <v>546</v>
+      </c>
+      <c r="C98" s="50" t="s">
+        <v>531</v>
+      </c>
+      <c r="D98" s="15" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="15" t="s">
+        <v>624</v>
+      </c>
+      <c r="B99" s="50" t="s">
+        <v>547</v>
+      </c>
+      <c r="C99" s="50" t="s">
+        <v>532</v>
+      </c>
+      <c r="D99" s="15" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="15" t="s">
+        <v>625</v>
+      </c>
+      <c r="B100" s="50" t="s">
+        <v>553</v>
+      </c>
+      <c r="C100" s="50" t="s">
+        <v>533</v>
+      </c>
+      <c r="D100" s="15" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="15" t="s">
+        <v>626</v>
+      </c>
+      <c r="B101" s="49" t="s">
+        <v>548</v>
+      </c>
+      <c r="C101" s="49" t="s">
+        <v>534</v>
+      </c>
+      <c r="D101" s="15" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="15" t="s">
+        <v>627</v>
+      </c>
+      <c r="B102" s="49" t="s">
+        <v>549</v>
+      </c>
+      <c r="C102" s="49" t="s">
+        <v>535</v>
+      </c>
+      <c r="D102" s="15" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="15" t="s">
+        <v>628</v>
+      </c>
+      <c r="B103" s="49" t="s">
+        <v>550</v>
+      </c>
+      <c r="C103" s="49" t="s">
+        <v>536</v>
+      </c>
+      <c r="D103" s="15" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="15" t="s">
+        <v>629</v>
+      </c>
+      <c r="B104" s="49" t="s">
+        <v>551</v>
+      </c>
+      <c r="C104" s="49" t="s">
+        <v>537</v>
+      </c>
+      <c r="D104" s="15" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="15" t="s">
+        <v>630</v>
+      </c>
+      <c r="B105" s="49" t="s">
+        <v>552</v>
+      </c>
+      <c r="C105" s="49" t="s">
+        <v>538</v>
+      </c>
+      <c r="D105" s="15" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="15" t="s">
+        <v>631</v>
+      </c>
+      <c r="B106" s="52" t="s">
+        <v>587</v>
+      </c>
+      <c r="C106" s="52" t="s">
+        <v>589</v>
+      </c>
+      <c r="D106" s="51" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="15" t="s">
+        <v>632</v>
+      </c>
+      <c r="B107" s="49" t="s">
+        <v>594</v>
+      </c>
+      <c r="C107" s="53" t="s">
+        <v>588</v>
+      </c>
+      <c r="D107" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="G107" s="11" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="15" t="s">
+        <v>633</v>
+      </c>
+      <c r="B108" s="52" t="s">
+        <v>595</v>
+      </c>
+      <c r="C108" s="52" t="s">
+        <v>591</v>
+      </c>
+      <c r="D108" s="15" t="s">
+        <v>592</v>
+      </c>
+      <c r="G108" s="11" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="15" t="s">
+        <v>634</v>
+      </c>
+      <c r="B109" s="49" t="s">
+        <v>596</v>
+      </c>
+      <c r="C109" s="49" t="s">
+        <v>597</v>
+      </c>
+      <c r="D109" s="49" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="15" t="s">
+        <v>635</v>
+      </c>
+      <c r="B110" s="15" t="s">
+        <v>571</v>
+      </c>
+      <c r="C110" s="15" t="s">
+        <v>572</v>
+      </c>
+      <c r="G110" s="11" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="15" t="s">
+        <v>636</v>
+      </c>
+      <c r="B111" s="46" t="s">
+        <v>570</v>
+      </c>
+      <c r="C111" s="46" t="s">
+        <v>567</v>
+      </c>
+      <c r="G111" s="11" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="15" t="s">
+        <v>637</v>
+      </c>
+      <c r="B112" s="50" t="s">
+        <v>563</v>
+      </c>
+      <c r="C112" s="50" t="s">
+        <v>564</v>
+      </c>
+      <c r="D112" s="50" t="s">
+        <v>567</v>
+      </c>
+      <c r="G112" s="11" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="15" t="s">
+        <v>638</v>
+      </c>
+      <c r="B113" s="46" t="s">
+        <v>569</v>
+      </c>
+      <c r="C113" s="46" t="s">
+        <v>566</v>
+      </c>
+      <c r="D113" s="46" t="s">
+        <v>567</v>
+      </c>
+      <c r="G113" s="11" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="15" t="s">
+        <v>639</v>
+      </c>
+      <c r="B114" s="15" t="s">
+        <v>568</v>
+      </c>
+      <c r="C114" s="15" t="s">
+        <v>565</v>
+      </c>
+      <c r="D114" s="46" t="s">
+        <v>566</v>
+      </c>
+      <c r="G114" s="11" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="15" t="s">
+        <v>640</v>
+      </c>
+      <c r="B115" s="46" t="s">
+        <v>573</v>
+      </c>
+      <c r="C115" s="46" t="s">
+        <v>574</v>
+      </c>
+      <c r="D115" s="15" t="s">
+        <v>565</v>
+      </c>
+      <c r="G115" s="11" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="15" t="s">
+        <v>641</v>
+      </c>
+      <c r="B116" s="46" t="s">
+        <v>575</v>
+      </c>
+      <c r="C116" s="46" t="s">
+        <v>576</v>
+      </c>
+      <c r="D116" s="46" t="s">
+        <v>574</v>
+      </c>
+      <c r="G116" s="11" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="15" t="s">
+        <v>642</v>
+      </c>
+      <c r="B117" s="46" t="s">
+        <v>577</v>
+      </c>
+      <c r="C117" s="46" t="s">
+        <v>554</v>
+      </c>
+      <c r="D117" s="46" t="s">
+        <v>578</v>
+      </c>
+      <c r="G117" s="11" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="15" t="s">
+        <v>643</v>
+      </c>
+      <c r="B118" s="50" t="s">
+        <v>598</v>
+      </c>
+      <c r="C118" s="50" t="s">
+        <v>599</v>
+      </c>
+      <c r="D118" s="50" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="15" t="s">
+        <v>644</v>
+      </c>
+      <c r="B119" s="50" t="s">
+        <v>600</v>
+      </c>
+      <c r="C119" s="50" t="s">
+        <v>601</v>
+      </c>
+      <c r="D119" s="50" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -7303,31 +8165,31 @@
   <sheetData>
     <row r="2" spans="1:2" ht="48" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>412</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="36" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>414</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -7351,72 +8213,72 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>
@@ -7452,7 +8314,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>1</v>
@@ -7511,46 +8373,46 @@
     </row>
     <row r="2" spans="1:20" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="C2" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>431</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>431</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>432</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>435</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>436</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>437</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="3" t="s">
         <v>43</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
   </sheetData>
@@ -7576,22 +8438,22 @@
     </row>
     <row r="22" spans="21:21" ht="60" x14ac:dyDescent="0.25">
       <c r="U22" s="12" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="24" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U24" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="27" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U27" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="28" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U28" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -7602,6 +8464,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="0c85289e-a0a4-4193-8a36-83840327cccf" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="48f24ce9-3fee-408f-adaa-6c70c8fcad88">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC0853FBA342F1439B1E03C364E3AF64" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b473cb13b29a9ff7b19694f6b2f73718">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="48f24ce9-3fee-408f-adaa-6c70c8fcad88" xmlns:ns3="0c85289e-a0a4-4193-8a36-83840327cccf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6fe4fbd77109f000862c0d72bea26d08" ns2:_="" ns3:_="">
     <xsd:import namespace="48f24ce9-3fee-408f-adaa-6c70c8fcad88"/>
@@ -7856,27 +8738,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="0c85289e-a0a4-4193-8a36-83840327cccf" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="48f24ce9-3fee-408f-adaa-6c70c8fcad88">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8CB4D6B-32F5-433C-B912-80588CDBA322}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="48f24ce9-3fee-408f-adaa-6c70c8fcad88"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="0c85289e-a0a4-4193-8a36-83840327cccf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E189810-EDFC-4989-8B68-DF434BA155E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85BC1396-D9DB-46DB-90A3-32A510C50206}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7895,27 +8782,8 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8CB4D6B-32F5-433C-B912-80588CDBA322}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="48f24ce9-3fee-408f-adaa-6c70c8fcad88"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="0c85289e-a0a4-4193-8a36-83840327cccf"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E189810-EDFC-4989-8B68-DF434BA155E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{14b77578-9773-42d5-8507-251ca2dc2b06}" enabled="0" method="" siteId="{14b77578-9773-42d5-8507-251ca2dc2b06}" removed="1"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
updates based on work around function-ing
</commit_message>
<xml_diff>
--- a/resources/OntologyTopLevelDefinitions.xlsx
+++ b/resources/OntologyTopLevelDefinitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\divitag2\work\softwareRepos\EcologicalMentalFunctioningOntology\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745472EE-537C-4F5B-9AC5-7C86023ADFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEEED22-81B5-4248-A699-E9EB5862480B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29430" yWindow="2535" windowWidth="26295" windowHeight="11940" tabRatio="463" xr2:uid="{9A7D1081-669E-4486-97AA-E16A917A201B}"/>
+    <workbookView xWindow="39240" yWindow="360" windowWidth="37020" windowHeight="19035" tabRatio="463" activeTab="3" xr2:uid="{9A7D1081-669E-4486-97AA-E16A917A201B}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="1" r:id="rId1"/>
@@ -3477,12 +3477,6 @@
 The physical and social aspects of one's immediate life space that the person interacts with and can influence.</t>
   </si>
   <si>
-    <t>ttd - change has-modifier to mental functioning,  to has-attribute to level of performance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ttd make relationship between observalbe behavior to level of performance as </t>
-  </si>
-  <si>
     <t xml:space="preserve">A domain ontology that covers mental functioning from the perspective of an external observer such as a clinician.  This ontology provides the framework for funcioning in the context of an environment, personal factors, for point-in-time observations and the ability to quantify and qualify those observations. </t>
   </si>
   <si>
@@ -4011,6 +4005,12 @@
   </si>
   <si>
     <t>Proximal_Contextual_Factors</t>
+  </si>
+  <si>
+    <t>occurrent</t>
+  </si>
+  <si>
+    <t>TTD: Update</t>
   </si>
 </sst>
 </file>
@@ -4328,7 +4328,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4400,9 +4400,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4422,9 +4419,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -4448,7 +4442,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4466,9 +4459,38 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -4862,22 +4884,21 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:W119"/>
+  <dimension ref="A1:W120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F76" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C81" sqref="C81"/>
+      <selection pane="bottomRight" activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="26.7109375" style="15" customWidth="1"/>
     <col min="3" max="3" width="51.140625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="15" customWidth="1"/>
+    <col min="4" max="5" width="24.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="11" customWidth="1"/>
     <col min="7" max="7" width="61.7109375" style="11" customWidth="1"/>
     <col min="8" max="8" width="67" style="15" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" style="15" customWidth="1"/>
@@ -4899,7 +4920,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>0</v>
@@ -4907,13 +4928,13 @@
       <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="14" t="s">
@@ -4970,19 +4991,19 @@
     </row>
     <row r="2" spans="1:23" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>496</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="11" t="s">
         <v>23</v>
       </c>
       <c r="G2" s="11" t="s">
@@ -5019,7 +5040,7 @@
     </row>
     <row r="3" spans="1:23" ht="153" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>28</v>
@@ -5027,11 +5048,11 @@
       <c r="C3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="16"/>
+      <c r="D3" s="17"/>
       <c r="E3" s="17" t="s">
-        <v>497</v>
-      </c>
-      <c r="F3" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>30</v>
       </c>
       <c r="G3" s="17" t="s">
@@ -5068,22 +5089,22 @@
     </row>
     <row r="4" spans="1:23" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B4" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>498</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="39"/>
+      <c r="G4" s="37"/>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
@@ -5103,18 +5124,18 @@
     </row>
     <row r="5" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B5" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>498</v>
-      </c>
-      <c r="E5" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="11" t="s">
         <v>39</v>
       </c>
       <c r="G5" s="11" t="s">
@@ -5142,19 +5163,19 @@
     </row>
     <row r="6" spans="1:23" s="16" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B6" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>499</v>
-      </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15" t="s">
+        <v>497</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="11" t="s">
         <v>45</v>
       </c>
       <c r="G6" s="11" t="s">
@@ -5195,18 +5216,18 @@
     </row>
     <row r="7" spans="1:23" ht="165.75" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>512</v>
-      </c>
-      <c r="E7" s="15" t="s">
+        <v>510</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G7" s="11" t="s">
@@ -5232,24 +5253,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" s="16" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>50</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>512</v>
-      </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15" t="s">
+        <v>510</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="37" t="s">
         <v>60</v>
       </c>
       <c r="H8" s="18"/>
@@ -5271,7 +5292,7 @@
     </row>
     <row r="9" spans="1:23" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>61</v>
@@ -5279,11 +5300,11 @@
       <c r="C9" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="11" t="s">
         <v>63</v>
       </c>
       <c r="G9" s="11" t="s">
@@ -5320,21 +5341,21 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>66</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>513</v>
-      </c>
-      <c r="E10" s="15" t="s">
+        <v>511</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="29" t="s">
         <v>69</v>
       </c>
       <c r="H10" s="20"/>
@@ -5344,19 +5365,19 @@
     </row>
     <row r="11" spans="1:23" ht="191.25" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>513</v>
-      </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16" t="s">
+        <v>511</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="17" t="s">
         <v>71</v>
       </c>
       <c r="G11" s="17" t="s">
@@ -5397,7 +5418,7 @@
     </row>
     <row r="12" spans="1:23" s="16" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>77</v>
@@ -5405,10 +5426,11 @@
       <c r="C12" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="D12" s="17"/>
+      <c r="E12" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="17" t="s">
         <v>79</v>
       </c>
       <c r="G12" s="17" t="s">
@@ -5456,25 +5478,25 @@
     </row>
     <row r="13" spans="1:23" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>514</v>
-      </c>
-      <c r="E13" s="15" t="s">
+        <v>512</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="11" t="s">
         <v>85</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>86</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11" t="s">
@@ -5499,22 +5521,22 @@
     </row>
     <row r="14" spans="1:23" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B14" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>514</v>
-      </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15" t="s">
+        <v>512</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="G14" s="39"/>
+      <c r="G14" s="37"/>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
@@ -5534,13 +5556,13 @@
     </row>
     <row r="15" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B15" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>90</v>
@@ -5548,7 +5570,7 @@
       <c r="F15" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="G15" s="39"/>
+      <c r="G15" s="37"/>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
@@ -5556,13 +5578,13 @@
     </row>
     <row r="16" spans="1:23" s="16" customFormat="1" ht="89.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B16" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11" t="s">
@@ -5609,7 +5631,7 @@
     </row>
     <row r="17" spans="1:23" ht="204" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>99</v>
@@ -5654,7 +5676,7 @@
     </row>
     <row r="18" spans="1:23" ht="242.25" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>106</v>
@@ -5662,15 +5684,15 @@
       <c r="C18" s="16" t="s">
         <v>404</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16" t="s">
+      <c r="D18" s="17"/>
+      <c r="E18" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="17" t="s">
         <v>108</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="H18" s="17" t="s">
         <v>109</v>
@@ -5707,7 +5729,7 @@
     </row>
     <row r="19" spans="1:23" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>112</v>
@@ -5715,8 +5737,8 @@
       <c r="C19" s="16" t="s">
         <v>372</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16" t="s">
+      <c r="D19" s="17"/>
+      <c r="E19" s="17" t="s">
         <v>107</v>
       </c>
       <c r="F19" s="24" t="s">
@@ -5760,7 +5782,7 @@
     </row>
     <row r="20" spans="1:23" s="16" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>117</v>
@@ -5768,10 +5790,11 @@
       <c r="C20" s="16" t="s">
         <v>118</v>
       </c>
+      <c r="D20" s="17"/>
       <c r="E20" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="17" t="s">
         <v>120</v>
       </c>
       <c r="G20" s="17" t="s">
@@ -5796,15 +5819,15 @@
     </row>
     <row r="21" spans="1:23" ht="51" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>124</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>501</v>
-      </c>
-      <c r="D21" s="16"/>
+        <v>499</v>
+      </c>
+      <c r="D21" s="17"/>
       <c r="E21" s="17" t="s">
         <v>125</v>
       </c>
@@ -5835,18 +5858,19 @@
     </row>
     <row r="22" spans="1:23" s="16" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B22" s="45" t="s">
-        <v>480</v>
+        <v>493</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>478</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>502</v>
-      </c>
-      <c r="E22" s="16" t="s">
+        <v>500</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="17" t="s">
         <v>130</v>
       </c>
       <c r="G22" s="17" t="s">
@@ -5880,7 +5904,7 @@
     </row>
     <row r="23" spans="1:23" s="20" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>136</v>
@@ -5908,7 +5932,7 @@
       <c r="K23" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="L23" s="25" t="s">
+      <c r="L23" s="24" t="s">
         <v>142</v>
       </c>
       <c r="M23" s="16"/>
@@ -5933,18 +5957,19 @@
     </row>
     <row r="24" spans="1:23" s="16" customFormat="1" ht="102" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B24" s="46" t="s">
-        <v>481</v>
+        <v>493</v>
+      </c>
+      <c r="B24" s="43" t="s">
+        <v>479</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>503</v>
-      </c>
-      <c r="E24" s="16" t="s">
+        <v>501</v>
+      </c>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="17" t="s">
         <v>144</v>
       </c>
       <c r="G24" s="17" t="s">
@@ -5969,15 +5994,15 @@
     </row>
     <row r="25" spans="1:23" ht="51" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B25" s="46" t="s">
-        <v>482</v>
+        <v>493</v>
+      </c>
+      <c r="B25" s="43" t="s">
+        <v>480</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>504</v>
-      </c>
-      <c r="D25" s="16"/>
+        <v>502</v>
+      </c>
+      <c r="D25" s="17"/>
       <c r="E25" s="17" t="s">
         <v>148</v>
       </c>
@@ -6020,18 +6045,19 @@
     </row>
     <row r="26" spans="1:23" s="16" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>153</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>505</v>
-      </c>
-      <c r="E26" s="16" t="s">
+        <v>503</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="17" t="s">
         <v>155</v>
       </c>
       <c r="G26" s="17" t="s">
@@ -6068,7 +6094,7 @@
     </row>
     <row r="27" spans="1:23" ht="102" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>160</v>
@@ -6076,13 +6102,13 @@
       <c r="C27" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="G27" s="25" t="s">
         <v>163</v>
       </c>
       <c r="H27" s="11" t="s">
@@ -6107,7 +6133,7 @@
     </row>
     <row r="28" spans="1:23" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>166</v>
@@ -6115,17 +6141,17 @@
       <c r="C28" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="11" t="s">
         <v>169</v>
       </c>
       <c r="G28" s="11" t="s">
         <v>170</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="I28" s="11"/>
       <c r="J28" s="11" t="s">
@@ -6149,29 +6175,29 @@
     </row>
     <row r="29" spans="1:23" s="16" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B29" s="46" t="s">
-        <v>483</v>
+        <v>493</v>
+      </c>
+      <c r="B29" s="43" t="s">
+        <v>481</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D29" s="17"/>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="17" t="s">
         <v>173</v>
       </c>
       <c r="G29" s="17" t="s">
         <v>174</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="I29" s="17"/>
-      <c r="J29" s="27" t="s">
+      <c r="J29" s="26" t="s">
         <v>175</v>
       </c>
       <c r="K29" s="17" t="s">
@@ -6195,18 +6221,18 @@
     </row>
     <row r="30" spans="1:23" ht="51" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B30" s="46" t="s">
-        <v>484</v>
+        <v>493</v>
+      </c>
+      <c r="B30" s="43" t="s">
+        <v>482</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>507</v>
-      </c>
-      <c r="E30" s="15" t="s">
+        <v>505</v>
+      </c>
+      <c r="E30" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="11" t="s">
         <v>179</v>
       </c>
       <c r="G30" s="11" t="s">
@@ -6237,18 +6263,19 @@
     </row>
     <row r="31" spans="1:23" s="16" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B31" s="46" t="s">
-        <v>485</v>
+        <v>493</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>483</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>508</v>
-      </c>
-      <c r="E31" s="16" t="s">
+        <v>506</v>
+      </c>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="F31" s="17" t="s">
         <v>184</v>
       </c>
       <c r="G31" s="17" t="s">
@@ -6279,7 +6306,7 @@
     </row>
     <row r="32" spans="1:23" ht="51" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>188</v>
@@ -6287,11 +6314,11 @@
       <c r="C32" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16" t="s">
+      <c r="D32" s="17"/>
+      <c r="E32" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="F32" s="17" t="s">
         <v>191</v>
       </c>
       <c r="G32" s="17" t="s">
@@ -6304,7 +6331,7 @@
       <c r="J32" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="K32" s="28" t="s">
+      <c r="K32" s="27" t="s">
         <v>43</v>
       </c>
       <c r="L32" s="17" t="s">
@@ -6328,7 +6355,7 @@
     </row>
     <row r="33" spans="1:23" s="16" customFormat="1" ht="102" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>196</v>
@@ -6336,11 +6363,11 @@
       <c r="C33" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15" t="s">
+      <c r="D33" s="11"/>
+      <c r="E33" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F33" s="11" t="s">
         <v>37</v>
       </c>
       <c r="G33" s="11" t="s">
@@ -6353,7 +6380,7 @@
       <c r="J33" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="K33" s="29" t="s">
+      <c r="K33" s="28" t="s">
         <v>200</v>
       </c>
       <c r="L33" s="15"/>
@@ -6377,33 +6404,33 @@
     </row>
     <row r="34" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="29" t="s">
         <v>202</v>
       </c>
-      <c r="D34" s="30"/>
-      <c r="E34" s="20" t="s">
+      <c r="D34" s="29"/>
+      <c r="E34" s="29" t="s">
         <v>203</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="F34" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="G34" s="30" t="s">
+      <c r="G34" s="29" t="s">
         <v>205</v>
       </c>
-      <c r="H34" s="30" t="s">
+      <c r="H34" s="29" t="s">
         <v>206</v>
       </c>
-      <c r="I34" s="30"/>
-      <c r="J34" s="31" t="s">
+      <c r="I34" s="29"/>
+      <c r="J34" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30" t="s">
+      <c r="K34" s="29"/>
+      <c r="L34" s="29" t="s">
         <v>208</v>
       </c>
       <c r="M34" s="20"/>
@@ -6420,7 +6447,7 @@
     </row>
     <row r="35" spans="1:23" s="16" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>209</v>
@@ -6428,10 +6455,11 @@
       <c r="C35" s="16" t="s">
         <v>343</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="D35" s="17"/>
+      <c r="E35" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="F35" s="17" t="s">
         <v>211</v>
       </c>
       <c r="G35" s="17" t="s">
@@ -6472,7 +6500,7 @@
     </row>
     <row r="36" spans="1:23" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B36" s="21" t="s">
         <v>209</v>
@@ -6480,7 +6508,7 @@
       <c r="C36" s="16" t="s">
         <v>343</v>
       </c>
-      <c r="D36" s="16"/>
+      <c r="D36" s="17"/>
       <c r="E36" s="17" t="s">
         <v>216</v>
       </c>
@@ -6513,18 +6541,18 @@
     </row>
     <row r="37" spans="1:23" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B37" s="45" t="s">
-        <v>486</v>
+        <v>493</v>
+      </c>
+      <c r="B37" s="42" t="s">
+        <v>484</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>509</v>
-      </c>
-      <c r="E37" s="15" t="s">
+        <v>507</v>
+      </c>
+      <c r="E37" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="F37" s="15" t="s">
+      <c r="F37" s="11" t="s">
         <v>221</v>
       </c>
       <c r="G37" s="11" t="s">
@@ -6555,18 +6583,19 @@
     </row>
     <row r="38" spans="1:23" s="16" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B38" s="45" t="s">
-        <v>487</v>
+        <v>493</v>
+      </c>
+      <c r="B38" s="42" t="s">
+        <v>485</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>510</v>
-      </c>
-      <c r="E38" s="16" t="s">
+        <v>508</v>
+      </c>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="F38" s="16" t="s">
+      <c r="F38" s="17" t="s">
         <v>227</v>
       </c>
       <c r="G38" s="17" t="s">
@@ -6600,18 +6629,18 @@
     </row>
     <row r="39" spans="1:23" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B39" s="46" t="s">
-        <v>488</v>
+        <v>493</v>
+      </c>
+      <c r="B39" s="43" t="s">
+        <v>486</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>511</v>
-      </c>
-      <c r="E39" s="32" t="s">
+        <v>509</v>
+      </c>
+      <c r="E39" s="50" t="s">
         <v>232</v>
       </c>
-      <c r="F39" s="32" t="s">
+      <c r="F39" s="50" t="s">
         <v>233</v>
       </c>
       <c r="G39" s="11" t="s">
@@ -6645,7 +6674,7 @@
     </row>
     <row r="40" spans="1:23" s="16" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B40" s="21" t="s">
         <v>239</v>
@@ -6653,6 +6682,9 @@
       <c r="C40" s="16" t="s">
         <v>240</v>
       </c>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
       <c r="G40" s="17" t="s">
         <v>241</v>
       </c>
@@ -6681,35 +6713,35 @@
     </row>
     <row r="41" spans="1:23" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B41" s="33" t="s">
+        <v>493</v>
+      </c>
+      <c r="B41" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="C41" s="33" t="s">
+      <c r="C41" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="D41" s="33" t="s">
+      <c r="D41" s="51" t="s">
         <v>247</v>
       </c>
-      <c r="G41" s="44" t="s">
-        <v>472</v>
-      </c>
-      <c r="H41" s="44" t="s">
-        <v>473</v>
+      <c r="G41" s="41" t="s">
+        <v>470</v>
+      </c>
+      <c r="H41" s="41" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="42" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B42" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B42" s="32" t="s">
         <v>248</v>
       </c>
-      <c r="C42" s="34" t="s">
+      <c r="C42" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="D42" s="34" t="s">
+      <c r="D42" s="33" t="s">
         <v>250</v>
       </c>
       <c r="G42" s="11" t="s">
@@ -6721,21 +6753,21 @@
     </row>
     <row r="43" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B43" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B43" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="C43" s="34" t="s">
+      <c r="C43" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="D43" s="34" t="s">
+      <c r="D43" s="33" t="s">
         <v>250</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="F43" s="15" t="s">
+      <c r="F43" s="11" t="s">
         <v>256</v>
       </c>
       <c r="G43" s="11" t="s">
@@ -6754,21 +6786,21 @@
     </row>
     <row r="44" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B44" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B44" s="32" t="s">
         <v>261</v>
       </c>
-      <c r="C44" s="34" t="s">
-        <v>559</v>
-      </c>
-      <c r="D44" s="34" t="s">
+      <c r="C44" s="32" t="s">
+        <v>557</v>
+      </c>
+      <c r="D44" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="E44" s="15" t="s">
+      <c r="E44" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="F44" s="11" t="s">
         <v>263</v>
       </c>
       <c r="G44" s="11" t="s">
@@ -6777,48 +6809,48 @@
     </row>
     <row r="45" spans="1:23" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B45" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B45" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="C45" s="34" t="s">
+      <c r="C45" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="D45" s="34" t="s">
+      <c r="D45" s="33" t="s">
         <v>267</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="E45" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="F45" s="15" t="s">
+      <c r="F45" s="11" t="s">
         <v>269</v>
       </c>
       <c r="G45" s="11" t="s">
         <v>270</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="I45" s="11"/>
     </row>
     <row r="46" spans="1:23" ht="51" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B46" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B46" s="32" t="s">
         <v>271</v>
       </c>
-      <c r="C46" s="34" t="s">
+      <c r="C46" s="32" t="s">
         <v>272</v>
       </c>
-      <c r="D46" s="34" t="s">
+      <c r="D46" s="33" t="s">
         <v>267</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="F46" s="15" t="s">
+      <c r="F46" s="11" t="s">
         <v>274</v>
       </c>
       <c r="G46" s="11" t="s">
@@ -6831,21 +6863,21 @@
     </row>
     <row r="47" spans="1:23" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B47" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B47" s="32" t="s">
         <v>277</v>
       </c>
-      <c r="C47" s="34" t="s">
+      <c r="C47" s="32" t="s">
         <v>278</v>
       </c>
-      <c r="D47" s="34" t="s">
+      <c r="D47" s="33" t="s">
         <v>267</v>
       </c>
-      <c r="E47" s="15" t="s">
+      <c r="E47" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="F47" s="41" t="s">
+      <c r="F47" s="52" t="s">
         <v>280</v>
       </c>
       <c r="G47" s="11" t="s">
@@ -6858,15 +6890,15 @@
     </row>
     <row r="48" spans="1:23" ht="51" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B48" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B48" s="32" t="s">
         <v>283</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="C48" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="D48" s="34" t="s">
+      <c r="D48" s="33" t="s">
         <v>267</v>
       </c>
       <c r="G48" s="11" t="s">
@@ -6879,15 +6911,15 @@
     </row>
     <row r="49" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B49" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B49" s="32" t="s">
         <v>287</v>
       </c>
-      <c r="C49" s="34" t="s">
+      <c r="C49" s="32" t="s">
         <v>288</v>
       </c>
-      <c r="D49" s="34" t="s">
+      <c r="D49" s="33" t="s">
         <v>267</v>
       </c>
       <c r="G49" s="11" t="s">
@@ -6900,15 +6932,15 @@
     </row>
     <row r="50" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B50" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B50" s="32" t="s">
         <v>291</v>
       </c>
-      <c r="C50" s="34" t="s">
+      <c r="C50" s="32" t="s">
         <v>292</v>
       </c>
-      <c r="D50" s="34" t="s">
+      <c r="D50" s="33" t="s">
         <v>267</v>
       </c>
       <c r="G50" s="11" t="s">
@@ -6921,15 +6953,15 @@
     </row>
     <row r="51" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B51" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B51" s="32" t="s">
         <v>295</v>
       </c>
-      <c r="C51" s="34" t="s">
+      <c r="C51" s="32" t="s">
         <v>296</v>
       </c>
-      <c r="D51" s="34" t="s">
+      <c r="D51" s="33" t="s">
         <v>267</v>
       </c>
       <c r="G51" s="11" t="s">
@@ -6942,15 +6974,15 @@
     </row>
     <row r="52" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B52" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B52" s="32" t="s">
         <v>299</v>
       </c>
-      <c r="C52" s="34" t="s">
+      <c r="C52" s="32" t="s">
         <v>300</v>
       </c>
-      <c r="D52" s="34" t="s">
+      <c r="D52" s="33" t="s">
         <v>267</v>
       </c>
       <c r="G52" s="11" t="s">
@@ -6963,18 +6995,17 @@
     </row>
     <row r="53" spans="1:9" ht="204" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B53" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B53" s="32" t="s">
         <v>303</v>
       </c>
-      <c r="C53" s="34" t="s">
+      <c r="C53" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="D53" s="34" t="s">
+      <c r="D53" s="33" t="s">
         <v>267</v>
       </c>
-      <c r="F53" s="11"/>
       <c r="G53" s="11" t="s">
         <v>305</v>
       </c>
@@ -6985,15 +7016,15 @@
     </row>
     <row r="54" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B54" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B54" s="32" t="s">
         <v>307</v>
       </c>
-      <c r="C54" s="34" t="s">
+      <c r="C54" s="32" t="s">
         <v>308</v>
       </c>
-      <c r="D54" s="34" t="s">
+      <c r="D54" s="33" t="s">
         <v>309</v>
       </c>
       <c r="G54" s="11" t="s">
@@ -7006,15 +7037,15 @@
     </row>
     <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B55" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B55" s="32" t="s">
         <v>312</v>
       </c>
-      <c r="C55" s="35" t="s">
+      <c r="C55" s="33" t="s">
         <v>313</v>
       </c>
-      <c r="D55" s="34" t="s">
+      <c r="D55" s="33" t="s">
         <v>314</v>
       </c>
       <c r="G55" s="11" t="s">
@@ -7024,17 +7055,17 @@
         <v>316</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B56" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B56" s="32" t="s">
         <v>317</v>
       </c>
-      <c r="C56" s="34" t="s">
+      <c r="C56" s="32" t="s">
         <v>318</v>
       </c>
-      <c r="D56" s="34" t="s">
+      <c r="D56" s="33" t="s">
         <v>314</v>
       </c>
       <c r="G56" s="11" t="s">
@@ -7043,15 +7074,15 @@
     </row>
     <row r="57" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B57" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B57" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="C57" s="34" t="s">
+      <c r="C57" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="D57" s="34" t="s">
+      <c r="D57" s="33" t="s">
         <v>314</v>
       </c>
       <c r="G57" s="11" t="s">
@@ -7063,15 +7094,15 @@
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B58" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B58" s="32" t="s">
         <v>324</v>
       </c>
-      <c r="C58" s="35" t="s">
+      <c r="C58" s="33" t="s">
         <v>325</v>
       </c>
-      <c r="D58" s="34" t="s">
+      <c r="D58" s="33" t="s">
         <v>314</v>
       </c>
       <c r="G58" s="11" t="s">
@@ -7083,15 +7114,15 @@
     </row>
     <row r="59" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B59" s="45" t="s">
-        <v>489</v>
-      </c>
-      <c r="C59" s="35" t="s">
-        <v>516</v>
-      </c>
-      <c r="D59" s="34"/>
+        <v>493</v>
+      </c>
+      <c r="B59" s="42" t="s">
+        <v>487</v>
+      </c>
+      <c r="C59" s="33" t="s">
+        <v>514</v>
+      </c>
+      <c r="D59" s="33"/>
       <c r="G59" s="11" t="s">
         <v>327</v>
       </c>
@@ -7101,15 +7132,15 @@
     </row>
     <row r="60" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B60" s="45" t="s">
-        <v>490</v>
-      </c>
-      <c r="C60" s="35" t="s">
-        <v>517</v>
-      </c>
-      <c r="D60" s="34"/>
+        <v>493</v>
+      </c>
+      <c r="B60" s="42" t="s">
+        <v>488</v>
+      </c>
+      <c r="C60" s="33" t="s">
+        <v>515</v>
+      </c>
+      <c r="D60" s="33"/>
       <c r="G60" s="11" t="s">
         <v>329</v>
       </c>
@@ -7119,45 +7150,45 @@
     </row>
     <row r="61" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B61" s="46" t="s">
-        <v>491</v>
-      </c>
-      <c r="C61" s="35" t="s">
-        <v>518</v>
-      </c>
-      <c r="D61" s="34"/>
+        <v>493</v>
+      </c>
+      <c r="B61" s="43" t="s">
+        <v>489</v>
+      </c>
+      <c r="C61" s="33" t="s">
+        <v>516</v>
+      </c>
+      <c r="D61" s="33"/>
       <c r="G61" s="11" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B62" s="46" t="s">
-        <v>492</v>
-      </c>
-      <c r="C62" s="35" t="s">
-        <v>519</v>
-      </c>
-      <c r="D62" s="34"/>
+        <v>493</v>
+      </c>
+      <c r="B62" s="43" t="s">
+        <v>490</v>
+      </c>
+      <c r="C62" s="33" t="s">
+        <v>517</v>
+      </c>
+      <c r="D62" s="33"/>
       <c r="G62" s="11" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B63" s="46" t="s">
         <v>493</v>
       </c>
-      <c r="C63" s="35" t="s">
-        <v>520</v>
-      </c>
-      <c r="D63" s="34"/>
+      <c r="B63" s="43" t="s">
+        <v>491</v>
+      </c>
+      <c r="C63" s="33" t="s">
+        <v>518</v>
+      </c>
+      <c r="D63" s="33"/>
       <c r="G63" s="11" t="s">
         <v>333</v>
       </c>
@@ -7165,17 +7196,17 @@
         <v>334</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B64" s="36" t="s">
+        <v>493</v>
+      </c>
+      <c r="B64" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="C64" s="36" t="s">
+      <c r="C64" s="34" t="s">
         <v>336</v>
       </c>
-      <c r="D64" s="36" t="s">
+      <c r="D64" s="53" t="s">
         <v>309</v>
       </c>
       <c r="E64" s="11" t="s">
@@ -7184,7 +7215,7 @@
       <c r="F64" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="G64" s="42" t="s">
+      <c r="G64" s="39" t="s">
         <v>339</v>
       </c>
       <c r="H64" s="11" t="s">
@@ -7193,21 +7224,21 @@
     </row>
     <row r="65" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B65" s="36" t="s">
+        <v>493</v>
+      </c>
+      <c r="B65" s="34" t="s">
         <v>341</v>
       </c>
-      <c r="C65" s="36" t="s">
+      <c r="C65" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D65" s="36" t="s">
+      <c r="D65" s="53" t="s">
         <v>343</v>
       </c>
-      <c r="E65" s="15" t="s">
+      <c r="E65" s="11" t="s">
         <v>441</v>
       </c>
-      <c r="F65" s="15" t="s">
+      <c r="F65" s="11" t="s">
         <v>440</v>
       </c>
       <c r="G65" s="11" t="s">
@@ -7219,45 +7250,45 @@
     </row>
     <row r="66" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B66" s="36" t="s">
+        <v>493</v>
+      </c>
+      <c r="B66" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="C66" s="36" t="s">
+      <c r="C66" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="D66" s="36" t="s">
+      <c r="D66" s="53" t="s">
         <v>343</v>
       </c>
-      <c r="E66" s="15" t="s">
+      <c r="E66" s="11" t="s">
         <v>442</v>
       </c>
-      <c r="F66" s="15" t="s">
+      <c r="F66" s="11" t="s">
         <v>443</v>
       </c>
       <c r="G66" s="11" t="s">
         <v>449</v>
       </c>
-      <c r="H66" s="43"/>
+      <c r="H66" s="40"/>
     </row>
     <row r="67" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B67" s="36" t="s">
+        <v>493</v>
+      </c>
+      <c r="B67" s="34" t="s">
         <v>348</v>
       </c>
-      <c r="C67" s="36" t="s">
+      <c r="C67" s="34" t="s">
         <v>349</v>
       </c>
-      <c r="D67" s="36" t="s">
+      <c r="D67" s="53" t="s">
         <v>350</v>
       </c>
-      <c r="E67" s="15" t="s">
+      <c r="E67" s="11" t="s">
         <v>451</v>
       </c>
-      <c r="F67" s="15" t="s">
+      <c r="F67" s="11" t="s">
         <v>450</v>
       </c>
       <c r="G67" s="11" t="s">
@@ -7269,41 +7300,41 @@
     </row>
     <row r="68" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B68" s="36" t="s">
+        <v>493</v>
+      </c>
+      <c r="B68" s="34" t="s">
         <v>351</v>
       </c>
-      <c r="C68" s="36" t="s">
+      <c r="C68" s="34" t="s">
         <v>352</v>
       </c>
-      <c r="D68" s="36" t="s">
+      <c r="D68" s="53" t="s">
         <v>353</v>
       </c>
-      <c r="E68" s="15" t="s">
+      <c r="E68" s="11" t="s">
         <v>354</v>
       </c>
-      <c r="F68" s="15" t="s">
+      <c r="F68" s="11" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B69" s="36" t="s">
+        <v>493</v>
+      </c>
+      <c r="B69" s="34" t="s">
         <v>356</v>
       </c>
-      <c r="C69" s="36" t="s">
+      <c r="C69" s="34" t="s">
         <v>357</v>
       </c>
-      <c r="D69" s="36" t="s">
+      <c r="D69" s="53" t="s">
         <v>352</v>
       </c>
-      <c r="E69" s="15" t="s">
+      <c r="E69" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="F69" s="15" t="s">
+      <c r="F69" s="11" t="s">
         <v>359</v>
       </c>
       <c r="G69" s="11" t="s">
@@ -7319,17 +7350,17 @@
         <v>363</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B70" s="36" t="s">
+        <v>493</v>
+      </c>
+      <c r="B70" s="34" t="s">
         <v>364</v>
       </c>
-      <c r="C70" s="36" t="s">
+      <c r="C70" s="34" t="s">
         <v>365</v>
       </c>
-      <c r="D70" s="36" t="s">
+      <c r="D70" s="53" t="s">
         <v>347</v>
       </c>
       <c r="G70" s="11" t="s">
@@ -7338,15 +7369,15 @@
     </row>
     <row r="71" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B71" s="36" t="s">
+        <v>493</v>
+      </c>
+      <c r="B71" s="34" t="s">
         <v>366</v>
       </c>
-      <c r="C71" s="36" t="s">
+      <c r="C71" s="34" t="s">
         <v>367</v>
       </c>
-      <c r="D71" s="36" t="s">
+      <c r="D71" s="53" t="s">
         <v>347</v>
       </c>
       <c r="G71" s="11" t="s">
@@ -7355,15 +7386,15 @@
     </row>
     <row r="72" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A72" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B72" s="36" t="s">
+        <v>493</v>
+      </c>
+      <c r="B72" s="34" t="s">
         <v>368</v>
       </c>
-      <c r="C72" s="36" t="s">
+      <c r="C72" s="34" t="s">
         <v>369</v>
       </c>
-      <c r="D72" s="36" t="s">
+      <c r="D72" s="53" t="s">
         <v>347</v>
       </c>
       <c r="G72" s="11" t="s">
@@ -7372,15 +7403,15 @@
     </row>
     <row r="73" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A73" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B73" s="37" t="s">
+        <v>493</v>
+      </c>
+      <c r="B73" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="C73" s="37" t="s">
+      <c r="C73" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="D73" s="37" t="s">
+      <c r="D73" s="54" t="s">
         <v>250</v>
       </c>
       <c r="G73" s="11" t="s">
@@ -7389,21 +7420,21 @@
     </row>
     <row r="74" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B74" s="37" t="s">
+        <v>493</v>
+      </c>
+      <c r="B74" s="35" t="s">
         <v>370</v>
       </c>
-      <c r="C74" s="37" t="s">
+      <c r="C74" s="35" t="s">
         <v>371</v>
       </c>
-      <c r="D74" s="37" t="s">
+      <c r="D74" s="54" t="s">
         <v>372</v>
       </c>
-      <c r="E74" s="15" t="s">
+      <c r="E74" s="11" t="s">
         <v>371</v>
       </c>
-      <c r="F74" s="15" t="s">
+      <c r="F74" s="11" t="s">
         <v>373</v>
       </c>
       <c r="G74" s="11" t="s">
@@ -7421,21 +7452,21 @@
     </row>
     <row r="75" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A75" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B75" s="37" t="s">
+        <v>493</v>
+      </c>
+      <c r="B75" s="35" t="s">
         <v>378</v>
       </c>
-      <c r="C75" s="37" t="s">
+      <c r="C75" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="D75" s="37" t="s">
+      <c r="D75" s="54" t="s">
         <v>372</v>
       </c>
-      <c r="E75" s="15" t="s">
+      <c r="E75" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="F75" s="15" t="s">
+      <c r="F75" s="11" t="s">
         <v>108</v>
       </c>
       <c r="G75" s="11" t="s">
@@ -7453,15 +7484,15 @@
     </row>
     <row r="76" spans="1:11" ht="102" x14ac:dyDescent="0.25">
       <c r="A76" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="B76" s="37" t="s">
+        <v>493</v>
+      </c>
+      <c r="B76" s="35" t="s">
         <v>381</v>
       </c>
-      <c r="C76" s="37" t="s">
-        <v>645</v>
-      </c>
-      <c r="D76" s="37" t="s">
+      <c r="C76" s="35" t="s">
+        <v>643</v>
+      </c>
+      <c r="D76" s="54" t="s">
         <v>383</v>
       </c>
       <c r="G76" s="11" t="s">
@@ -7473,15 +7504,15 @@
     </row>
     <row r="77" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
-        <v>602</v>
-      </c>
-      <c r="B77" s="37" t="s">
+        <v>600</v>
+      </c>
+      <c r="B77" s="35" t="s">
         <v>384</v>
       </c>
-      <c r="C77" s="37" t="s">
+      <c r="C77" s="35" t="s">
         <v>385</v>
       </c>
-      <c r="D77" s="37" t="s">
+      <c r="D77" s="54" t="s">
         <v>383</v>
       </c>
       <c r="G77" s="11" t="s">
@@ -7493,15 +7524,15 @@
     </row>
     <row r="78" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
-        <v>603</v>
-      </c>
-      <c r="B78" s="37" t="s">
+        <v>601</v>
+      </c>
+      <c r="B78" s="35" t="s">
         <v>388</v>
       </c>
-      <c r="C78" s="37" t="s">
+      <c r="C78" s="35" t="s">
         <v>389</v>
       </c>
-      <c r="D78" s="37" t="s">
+      <c r="D78" s="54" t="s">
         <v>382</v>
       </c>
       <c r="G78" s="11" t="s">
@@ -7510,15 +7541,15 @@
     </row>
     <row r="79" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="16" t="s">
-        <v>604</v>
-      </c>
-      <c r="B79" s="37" t="s">
+        <v>602</v>
+      </c>
+      <c r="B79" s="35" t="s">
         <v>390</v>
       </c>
-      <c r="C79" s="37" t="s">
+      <c r="C79" s="35" t="s">
         <v>391</v>
       </c>
-      <c r="D79" s="37" t="s">
+      <c r="D79" s="54" t="s">
         <v>382</v>
       </c>
       <c r="G79" s="11" t="s">
@@ -7527,15 +7558,15 @@
     </row>
     <row r="80" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A80" s="16" t="s">
-        <v>605</v>
-      </c>
-      <c r="B80" s="37" t="s">
+        <v>603</v>
+      </c>
+      <c r="B80" s="35" t="s">
         <v>392</v>
       </c>
-      <c r="C80" s="37" t="s">
+      <c r="C80" s="35" t="s">
         <v>393</v>
       </c>
-      <c r="D80" s="37" t="s">
+      <c r="D80" s="54" t="s">
         <v>382</v>
       </c>
       <c r="G80" s="11" t="s">
@@ -7547,15 +7578,15 @@
     </row>
     <row r="81" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
-        <v>606</v>
-      </c>
-      <c r="B81" s="37" t="s">
+        <v>604</v>
+      </c>
+      <c r="B81" s="35" t="s">
         <v>394</v>
       </c>
-      <c r="C81" s="37" t="s">
-        <v>646</v>
-      </c>
-      <c r="D81" s="37" t="s">
+      <c r="C81" s="35" t="s">
+        <v>644</v>
+      </c>
+      <c r="D81" s="54" t="s">
         <v>383</v>
       </c>
       <c r="G81" s="11" t="s">
@@ -7567,15 +7598,15 @@
     </row>
     <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="16" t="s">
-        <v>607</v>
-      </c>
-      <c r="B82" s="37" t="s">
+        <v>605</v>
+      </c>
+      <c r="B82" s="35" t="s">
         <v>396</v>
       </c>
-      <c r="C82" s="37" t="s">
+      <c r="C82" s="35" t="s">
         <v>397</v>
       </c>
-      <c r="D82" s="37" t="s">
+      <c r="D82" s="54" t="s">
         <v>395</v>
       </c>
       <c r="G82" s="11" t="s">
@@ -7587,15 +7618,15 @@
     </row>
     <row r="83" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A83" s="16" t="s">
-        <v>608</v>
-      </c>
-      <c r="B83" s="37" t="s">
+        <v>606</v>
+      </c>
+      <c r="B83" s="35" t="s">
         <v>398</v>
       </c>
-      <c r="C83" s="37" t="s">
+      <c r="C83" s="35" t="s">
         <v>399</v>
       </c>
-      <c r="D83" s="37" t="s">
+      <c r="D83" s="54" t="s">
         <v>395</v>
       </c>
       <c r="G83" s="11" t="s">
@@ -7604,15 +7635,15 @@
     </row>
     <row r="84" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="16" t="s">
-        <v>609</v>
-      </c>
-      <c r="B84" s="37" t="s">
+        <v>607</v>
+      </c>
+      <c r="B84" s="35" t="s">
         <v>400</v>
       </c>
-      <c r="C84" s="37" t="s">
+      <c r="C84" s="35" t="s">
         <v>401</v>
       </c>
-      <c r="D84" s="37" t="s">
+      <c r="D84" s="54" t="s">
         <v>395</v>
       </c>
       <c r="G84" s="11" t="s">
@@ -7621,15 +7652,15 @@
     </row>
     <row r="85" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="16" t="s">
-        <v>610</v>
-      </c>
-      <c r="B85" s="37" t="s">
+        <v>608</v>
+      </c>
+      <c r="B85" s="35" t="s">
         <v>402</v>
       </c>
-      <c r="C85" s="37" t="s">
+      <c r="C85" s="35" t="s">
         <v>403</v>
       </c>
-      <c r="D85" s="37" t="s">
+      <c r="D85" s="54" t="s">
         <v>404</v>
       </c>
       <c r="H85" s="15" t="s">
@@ -7638,15 +7669,15 @@
     </row>
     <row r="86" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="16" t="s">
-        <v>611</v>
-      </c>
-      <c r="B86" s="37" t="s">
+        <v>609</v>
+      </c>
+      <c r="B86" s="35" t="s">
         <v>405</v>
       </c>
-      <c r="C86" s="37" t="s">
+      <c r="C86" s="35" t="s">
         <v>406</v>
       </c>
-      <c r="D86" s="37" t="s">
+      <c r="D86" s="54" t="s">
         <v>404</v>
       </c>
       <c r="H86" s="15" t="s">
@@ -7655,488 +7686,493 @@
     </row>
     <row r="87" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="16" t="s">
-        <v>612</v>
-      </c>
-      <c r="B87" s="38" t="s">
+        <v>610</v>
+      </c>
+      <c r="B87" s="36" t="s">
         <v>407</v>
       </c>
-      <c r="C87" s="38" t="s">
+      <c r="C87" s="36" t="s">
         <v>408</v>
       </c>
-      <c r="D87" s="38" t="s">
+      <c r="D87" s="55" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="16" t="s">
-        <v>613</v>
-      </c>
-      <c r="B88" s="38" t="s">
+        <v>611</v>
+      </c>
+      <c r="B88" s="36" t="s">
         <v>409</v>
       </c>
-      <c r="C88" s="38" t="s">
+      <c r="C88" s="36" t="s">
         <v>410</v>
       </c>
-      <c r="D88" s="38" t="s">
+      <c r="D88" s="55" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
-        <v>614</v>
-      </c>
-      <c r="B89" s="47" t="s">
-        <v>539</v>
-      </c>
-      <c r="C89" s="47" t="s">
-        <v>556</v>
-      </c>
-      <c r="D89" s="46" t="s">
+        <v>612</v>
+      </c>
+      <c r="B89" s="44" t="s">
+        <v>537</v>
+      </c>
+      <c r="C89" s="44" t="s">
         <v>554</v>
+      </c>
+      <c r="D89" s="56" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
-        <v>615</v>
-      </c>
-      <c r="B90" s="47" t="s">
-        <v>540</v>
-      </c>
-      <c r="C90" s="47" t="s">
-        <v>525</v>
-      </c>
-      <c r="D90" s="15" t="s">
-        <v>555</v>
+        <v>613</v>
+      </c>
+      <c r="B90" s="44" t="s">
+        <v>538</v>
+      </c>
+      <c r="C90" s="44" t="s">
+        <v>523</v>
+      </c>
+      <c r="D90" s="11" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
-        <v>616</v>
-      </c>
-      <c r="B91" s="47" t="s">
-        <v>541</v>
-      </c>
-      <c r="C91" s="47" t="s">
-        <v>526</v>
-      </c>
-      <c r="D91" s="15" t="s">
+        <v>614</v>
+      </c>
+      <c r="B91" s="44" t="s">
+        <v>539</v>
+      </c>
+      <c r="C91" s="44" t="s">
+        <v>524</v>
+      </c>
+      <c r="D91" s="11" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
-        <v>617</v>
-      </c>
-      <c r="B92" s="47" t="s">
-        <v>542</v>
-      </c>
-      <c r="C92" s="47" t="s">
-        <v>527</v>
-      </c>
-      <c r="D92" s="15" t="s">
-        <v>526</v>
+        <v>615</v>
+      </c>
+      <c r="B92" s="44" t="s">
+        <v>540</v>
+      </c>
+      <c r="C92" s="44" t="s">
+        <v>525</v>
+      </c>
+      <c r="D92" s="11" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
-        <v>618</v>
-      </c>
-      <c r="B93" s="48" t="s">
-        <v>543</v>
-      </c>
-      <c r="C93" s="48" t="s">
-        <v>528</v>
-      </c>
-      <c r="D93" s="15" t="s">
+        <v>616</v>
+      </c>
+      <c r="B93" s="45" t="s">
+        <v>541</v>
+      </c>
+      <c r="C93" s="45" t="s">
         <v>526</v>
+      </c>
+      <c r="D93" s="11" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
-        <v>619</v>
-      </c>
-      <c r="B94" s="48" t="s">
-        <v>544</v>
-      </c>
-      <c r="C94" s="48" t="s">
-        <v>529</v>
-      </c>
-      <c r="D94" s="15" t="s">
-        <v>526</v>
+        <v>617</v>
+      </c>
+      <c r="B94" s="45" t="s">
+        <v>542</v>
+      </c>
+      <c r="C94" s="45" t="s">
+        <v>527</v>
+      </c>
+      <c r="D94" s="11" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
-        <v>620</v>
-      </c>
-      <c r="B95" s="48" t="s">
+        <v>618</v>
+      </c>
+      <c r="B95" s="45" t="s">
+        <v>555</v>
+      </c>
+      <c r="C95" s="45" t="s">
+        <v>556</v>
+      </c>
+      <c r="D95" s="11" t="s">
         <v>557</v>
-      </c>
-      <c r="C95" s="48" t="s">
-        <v>558</v>
-      </c>
-      <c r="D95" s="15" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
-        <v>621</v>
-      </c>
-      <c r="B96" s="48" t="s">
-        <v>561</v>
-      </c>
-      <c r="C96" s="48" t="s">
-        <v>560</v>
-      </c>
-      <c r="D96" s="15" t="s">
+        <v>619</v>
+      </c>
+      <c r="B96" s="45" t="s">
         <v>559</v>
+      </c>
+      <c r="C96" s="45" t="s">
+        <v>558</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
-        <v>622</v>
-      </c>
-      <c r="B97" s="49" t="s">
-        <v>545</v>
-      </c>
-      <c r="C97" s="49" t="s">
-        <v>530</v>
-      </c>
-      <c r="D97" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="B97" s="46" t="s">
+        <v>543</v>
+      </c>
+      <c r="C97" s="46" t="s">
+        <v>528</v>
+      </c>
+      <c r="D97" s="11" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
-        <v>623</v>
-      </c>
-      <c r="B98" s="50" t="s">
-        <v>546</v>
-      </c>
-      <c r="C98" s="50" t="s">
-        <v>531</v>
-      </c>
-      <c r="D98" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B98" s="47" t="s">
+        <v>544</v>
+      </c>
+      <c r="C98" s="47" t="s">
+        <v>529</v>
+      </c>
+      <c r="D98" s="11" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
-        <v>624</v>
-      </c>
-      <c r="B99" s="50" t="s">
-        <v>547</v>
-      </c>
-      <c r="C99" s="50" t="s">
-        <v>532</v>
-      </c>
-      <c r="D99" s="15" t="s">
-        <v>531</v>
+        <v>622</v>
+      </c>
+      <c r="B99" s="47" t="s">
+        <v>545</v>
+      </c>
+      <c r="C99" s="47" t="s">
+        <v>530</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
-        <v>625</v>
-      </c>
-      <c r="B100" s="50" t="s">
-        <v>553</v>
-      </c>
-      <c r="C100" s="50" t="s">
-        <v>533</v>
-      </c>
-      <c r="D100" s="15" t="s">
+        <v>623</v>
+      </c>
+      <c r="B100" s="47" t="s">
+        <v>551</v>
+      </c>
+      <c r="C100" s="47" t="s">
         <v>531</v>
+      </c>
+      <c r="D100" s="11" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
-        <v>626</v>
-      </c>
-      <c r="B101" s="49" t="s">
-        <v>548</v>
-      </c>
-      <c r="C101" s="49" t="s">
-        <v>534</v>
-      </c>
-      <c r="D101" s="15" t="s">
+        <v>624</v>
+      </c>
+      <c r="B101" s="46" t="s">
+        <v>546</v>
+      </c>
+      <c r="C101" s="46" t="s">
+        <v>532</v>
+      </c>
+      <c r="D101" s="11" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
-        <v>627</v>
-      </c>
-      <c r="B102" s="49" t="s">
-        <v>549</v>
-      </c>
-      <c r="C102" s="49" t="s">
-        <v>535</v>
-      </c>
-      <c r="D102" s="15" t="s">
-        <v>534</v>
+        <v>625</v>
+      </c>
+      <c r="B102" s="46" t="s">
+        <v>547</v>
+      </c>
+      <c r="C102" s="46" t="s">
+        <v>533</v>
+      </c>
+      <c r="D102" s="11" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
-        <v>628</v>
-      </c>
-      <c r="B103" s="49" t="s">
-        <v>550</v>
-      </c>
-      <c r="C103" s="49" t="s">
-        <v>536</v>
-      </c>
-      <c r="D103" s="15" t="s">
+        <v>626</v>
+      </c>
+      <c r="B103" s="46" t="s">
+        <v>548</v>
+      </c>
+      <c r="C103" s="46" t="s">
         <v>534</v>
+      </c>
+      <c r="D103" s="11" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
-        <v>629</v>
-      </c>
-      <c r="B104" s="49" t="s">
-        <v>551</v>
-      </c>
-      <c r="C104" s="49" t="s">
-        <v>537</v>
-      </c>
-      <c r="D104" s="15" t="s">
-        <v>534</v>
+        <v>627</v>
+      </c>
+      <c r="B104" s="46" t="s">
+        <v>549</v>
+      </c>
+      <c r="C104" s="46" t="s">
+        <v>535</v>
+      </c>
+      <c r="D104" s="11" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
-        <v>630</v>
-      </c>
-      <c r="B105" s="49" t="s">
-        <v>552</v>
-      </c>
-      <c r="C105" s="49" t="s">
-        <v>538</v>
-      </c>
-      <c r="D105" s="15" t="s">
-        <v>534</v>
+        <v>628</v>
+      </c>
+      <c r="B105" s="46" t="s">
+        <v>550</v>
+      </c>
+      <c r="C105" s="46" t="s">
+        <v>536</v>
+      </c>
+      <c r="D105" s="11" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
-        <v>631</v>
-      </c>
-      <c r="B106" s="52" t="s">
+        <v>629</v>
+      </c>
+      <c r="B106" s="48" t="s">
+        <v>585</v>
+      </c>
+      <c r="C106" s="48" t="s">
         <v>587</v>
       </c>
-      <c r="C106" s="52" t="s">
-        <v>589</v>
-      </c>
-      <c r="D106" s="51" t="s">
+      <c r="D106" s="57" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="15" t="s">
-        <v>632</v>
-      </c>
-      <c r="B107" s="49" t="s">
-        <v>594</v>
-      </c>
-      <c r="C107" s="53" t="s">
+        <v>630</v>
+      </c>
+      <c r="B107" s="46" t="s">
+        <v>592</v>
+      </c>
+      <c r="C107" s="49" t="s">
+        <v>586</v>
+      </c>
+      <c r="D107" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="G107" s="11" t="s">
         <v>588</v>
-      </c>
-      <c r="D107" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="G107" s="11" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="15" t="s">
-        <v>633</v>
-      </c>
-      <c r="B108" s="52" t="s">
-        <v>595</v>
-      </c>
-      <c r="C108" s="52" t="s">
+        <v>631</v>
+      </c>
+      <c r="B108" s="48" t="s">
+        <v>593</v>
+      </c>
+      <c r="C108" s="48" t="s">
+        <v>589</v>
+      </c>
+      <c r="D108" s="11" t="s">
+        <v>590</v>
+      </c>
+      <c r="G108" s="11" t="s">
         <v>591</v>
-      </c>
-      <c r="D108" s="15" t="s">
-        <v>592</v>
-      </c>
-      <c r="G108" s="11" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="15" t="s">
-        <v>634</v>
-      </c>
-      <c r="B109" s="49" t="s">
-        <v>596</v>
-      </c>
-      <c r="C109" s="49" t="s">
-        <v>597</v>
-      </c>
-      <c r="D109" s="49" t="s">
-        <v>562</v>
+        <v>632</v>
+      </c>
+      <c r="B109" s="46" t="s">
+        <v>594</v>
+      </c>
+      <c r="C109" s="46" t="s">
+        <v>595</v>
+      </c>
+      <c r="D109" s="58" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="15" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="G110" s="11" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="15" t="s">
-        <v>636</v>
-      </c>
-      <c r="B111" s="46" t="s">
-        <v>570</v>
-      </c>
-      <c r="C111" s="46" t="s">
-        <v>567</v>
+        <v>634</v>
+      </c>
+      <c r="B111" s="43" t="s">
+        <v>568</v>
+      </c>
+      <c r="C111" s="43" t="s">
+        <v>565</v>
       </c>
       <c r="G111" s="11" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="15" t="s">
-        <v>637</v>
-      </c>
-      <c r="B112" s="50" t="s">
-        <v>563</v>
-      </c>
-      <c r="C112" s="50" t="s">
-        <v>564</v>
-      </c>
-      <c r="D112" s="50" t="s">
-        <v>567</v>
+        <v>635</v>
+      </c>
+      <c r="B112" s="47" t="s">
+        <v>561</v>
+      </c>
+      <c r="C112" s="47" t="s">
+        <v>562</v>
+      </c>
+      <c r="D112" s="59" t="s">
+        <v>565</v>
       </c>
       <c r="G112" s="11" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="15" t="s">
-        <v>638</v>
-      </c>
-      <c r="B113" s="46" t="s">
-        <v>569</v>
-      </c>
-      <c r="C113" s="46" t="s">
-        <v>566</v>
-      </c>
-      <c r="D113" s="46" t="s">
+        <v>636</v>
+      </c>
+      <c r="B113" s="43" t="s">
         <v>567</v>
       </c>
+      <c r="C113" s="43" t="s">
+        <v>564</v>
+      </c>
+      <c r="D113" s="56" t="s">
+        <v>565</v>
+      </c>
       <c r="G113" s="11" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="15" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>565</v>
-      </c>
-      <c r="D114" s="46" t="s">
-        <v>566</v>
+        <v>563</v>
+      </c>
+      <c r="D114" s="56" t="s">
+        <v>564</v>
       </c>
       <c r="G114" s="11" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="15" t="s">
-        <v>640</v>
-      </c>
-      <c r="B115" s="46" t="s">
-        <v>573</v>
-      </c>
-      <c r="C115" s="46" t="s">
-        <v>574</v>
-      </c>
-      <c r="D115" s="15" t="s">
-        <v>565</v>
+        <v>638</v>
+      </c>
+      <c r="B115" s="43" t="s">
+        <v>571</v>
+      </c>
+      <c r="C115" s="43" t="s">
+        <v>572</v>
+      </c>
+      <c r="D115" s="11" t="s">
+        <v>563</v>
       </c>
       <c r="G115" s="11" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="15" t="s">
-        <v>641</v>
-      </c>
-      <c r="B116" s="46" t="s">
-        <v>575</v>
-      </c>
-      <c r="C116" s="46" t="s">
-        <v>576</v>
-      </c>
-      <c r="D116" s="46" t="s">
+        <v>639</v>
+      </c>
+      <c r="B116" s="43" t="s">
+        <v>573</v>
+      </c>
+      <c r="C116" s="43" t="s">
         <v>574</v>
       </c>
+      <c r="D116" s="56" t="s">
+        <v>572</v>
+      </c>
       <c r="G116" s="11" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
-        <v>642</v>
-      </c>
-      <c r="B117" s="46" t="s">
-        <v>577</v>
-      </c>
-      <c r="C117" s="46" t="s">
-        <v>554</v>
-      </c>
-      <c r="D117" s="46" t="s">
-        <v>578</v>
+        <v>640</v>
+      </c>
+      <c r="B117" s="43" t="s">
+        <v>575</v>
+      </c>
+      <c r="C117" s="43" t="s">
+        <v>552</v>
+      </c>
+      <c r="D117" s="56" t="s">
+        <v>576</v>
       </c>
       <c r="G117" s="11" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="15" t="s">
-        <v>643</v>
-      </c>
-      <c r="B118" s="50" t="s">
-        <v>598</v>
-      </c>
-      <c r="C118" s="50" t="s">
-        <v>599</v>
-      </c>
-      <c r="D118" s="50" t="s">
+        <v>641</v>
+      </c>
+      <c r="B118" s="47" t="s">
+        <v>596</v>
+      </c>
+      <c r="C118" s="47" t="s">
+        <v>597</v>
+      </c>
+      <c r="D118" s="59" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="15" t="s">
-        <v>644</v>
-      </c>
-      <c r="B119" s="50" t="s">
-        <v>600</v>
-      </c>
-      <c r="C119" s="50" t="s">
-        <v>601</v>
-      </c>
-      <c r="D119" s="50" t="s">
+        <v>642</v>
+      </c>
+      <c r="B119" s="47" t="s">
+        <v>598</v>
+      </c>
+      <c r="C119" s="47" t="s">
+        <v>599</v>
+      </c>
+      <c r="D119" s="59" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C120" s="15" t="s">
+        <v>645</v>
       </c>
     </row>
   </sheetData>
@@ -8153,7 +8189,7 @@
   <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8203,7 +8239,7 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8293,8 +8329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5FB70F-F965-4AC6-9CC3-9DF903077852}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8422,10 +8458,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5D464D-8C07-4FCB-A715-2D5BA637BEDD}">
-  <dimension ref="U2:U28"/>
+  <dimension ref="U2:U25"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="U29" sqref="U29"/>
+      <selection activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8434,7 +8470,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="21:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="U2" s="40"/>
+      <c r="U2" s="38"/>
     </row>
     <row r="22" spans="21:21" ht="60" x14ac:dyDescent="0.25">
       <c r="U22" s="12" t="s">
@@ -8446,14 +8482,9 @@
         <v>439</v>
       </c>
     </row>
-    <row r="27" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U27" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="28" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U28" t="s">
-        <v>471</v>
+    <row r="25" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U25" t="s">
+        <v>646</v>
       </c>
     </row>
   </sheetData>
@@ -8464,6 +8495,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="0c85289e-a0a4-4193-8a36-83840327cccf" xsi:nil="true"/>
@@ -8472,15 +8512,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8739,26 +8770,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8CB4D6B-32F5-433C-B912-80588CDBA322}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E189810-EDFC-4989-8B68-DF434BA155E0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="48f24ce9-3fee-408f-adaa-6c70c8fcad88"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="0c85289e-a0a4-4193-8a36-83840327cccf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E189810-EDFC-4989-8B68-DF434BA155E0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8CB4D6B-32F5-433C-B912-80588CDBA322}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="48f24ce9-3fee-408f-adaa-6c70c8fcad88"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="0c85289e-a0a4-4193-8a36-83840327cccf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>